<commit_message>
CTECH-887 Update sheets to reflect column changes
</commit_message>
<xml_diff>
--- a/LUSID Excel - Manage instruments with economic definitions.xlsx
+++ b/LUSID Excel - Manage instruments with economic definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2CBBF2-F06C-4DC1-955B-35B6F4DFD530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DD4811-088C-4500-8B5F-34E374E521ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{610DF3B5-2DE7-41D6-946E-DDB270968A5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{610DF3B5-2DE7-41D6-946E-DDB270968A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="FxForwards" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>This sheet allows you to:</t>
   </si>
@@ -88,12 +88,6 @@
   </si>
   <si>
     <t>Instrument Ids</t>
-  </si>
-  <si>
-    <t>LookThroughPortfolioId Scope</t>
-  </si>
-  <si>
-    <t>LookThroughPortfolioId Code</t>
   </si>
   <si>
     <t>StartDate</t>
@@ -199,9 +193,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -316,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -328,13 +319,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -358,498 +343,498 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.18df948ffd4747e49d738fb50ed12bec">
+    <main first="rtdsrv.9ab47963834640bc914c733d5ccad4d8">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>af43bf5d-e2f3-4973-9fa8-962672089b30</stp>
+        <stp>f4456094-26c6-4647-beed-513e0c6fc7a2</stp>
+        <tr r="L23" s="2"/>
+        <tr r="R27" s="2"/>
+        <tr r="S19" s="2"/>
+        <tr r="K21" s="2"/>
+        <tr r="O16" s="2"/>
+        <tr r="V23" s="2"/>
+        <tr r="I17" s="2"/>
+        <tr r="L16" s="2"/>
+        <tr r="V24" s="2"/>
+        <tr r="E18" s="2"/>
+        <tr r="W19" s="2"/>
+        <tr r="O21" s="2"/>
+        <tr r="O27" s="2"/>
+        <tr r="Z24" s="2"/>
+        <tr r="D26" s="2"/>
+        <tr r="X23" s="2"/>
+        <tr r="D27" s="2"/>
+        <tr r="S24" s="2"/>
+        <tr r="X17" s="2"/>
+        <tr r="Y24" s="2"/>
+        <tr r="R24" s="2"/>
+        <tr r="P24" s="2"/>
+        <tr r="AA20" s="2"/>
+        <tr r="S25" s="2"/>
+        <tr r="U19" s="2"/>
+        <tr r="M21" s="2"/>
+        <tr r="J25" s="2"/>
+        <tr r="J20" s="2"/>
+        <tr r="C23" s="2"/>
+        <tr r="K19" s="2"/>
+        <tr r="I19" s="2"/>
+        <tr r="F19" s="2"/>
+        <tr r="W24" s="2"/>
+        <tr r="C22" s="2"/>
+        <tr r="V17" s="2"/>
+        <tr r="AA18" s="2"/>
+        <tr r="Z27" s="2"/>
+        <tr r="Y22" s="2"/>
+        <tr r="P22" s="2"/>
+        <tr r="G26" s="2"/>
+        <tr r="Y26" s="2"/>
+        <tr r="P25" s="2"/>
+        <tr r="M25" s="2"/>
+        <tr r="T23" s="2"/>
+        <tr r="P20" s="2"/>
+        <tr r="S27" s="2"/>
+        <tr r="T27" s="2"/>
+        <tr r="T17" s="2"/>
+        <tr r="AA22" s="2"/>
+        <tr r="K22" s="2"/>
+        <tr r="V21" s="2"/>
+        <tr r="L17" s="2"/>
+        <tr r="AA21" s="2"/>
+        <tr r="C19" s="2"/>
+        <tr r="Q22" s="2"/>
+        <tr r="V22" s="2"/>
+        <tr r="D19" s="2"/>
+        <tr r="Z25" s="2"/>
+        <tr r="M18" s="2"/>
+        <tr r="O20" s="2"/>
+        <tr r="Y20" s="2"/>
+        <tr r="D17" s="2"/>
+        <tr r="R26" s="2"/>
+        <tr r="V26" s="2"/>
+        <tr r="S21" s="2"/>
+        <tr r="W20" s="2"/>
+        <tr r="J27" s="2"/>
+        <tr r="M24" s="2"/>
+        <tr r="Z20" s="2"/>
+        <tr r="S16" s="2"/>
+        <tr r="C27" s="2"/>
+        <tr r="P16" s="2"/>
+        <tr r="E23" s="2"/>
+        <tr r="H25" s="2"/>
+        <tr r="W23" s="2"/>
+        <tr r="J18" s="2"/>
+        <tr r="W16" s="2"/>
+        <tr r="U21" s="2"/>
+        <tr r="I18" s="2"/>
+        <tr r="F20" s="2"/>
+        <tr r="N26" s="2"/>
+        <tr r="K18" s="2"/>
+        <tr r="H21" s="2"/>
+        <tr r="U20" s="2"/>
+        <tr r="Q17" s="2"/>
+        <tr r="J26" s="2"/>
+        <tr r="N17" s="2"/>
+        <tr r="Y17" s="2"/>
+        <tr r="E19" s="2"/>
+        <tr r="F22" s="2"/>
+        <tr r="E17" s="2"/>
+        <tr r="H16" s="2"/>
+        <tr r="P26" s="2"/>
+        <tr r="L19" s="2"/>
+        <tr r="M23" s="2"/>
+        <tr r="U18" s="2"/>
+        <tr r="P27" s="2"/>
+        <tr r="L27" s="2"/>
+        <tr r="AA24" s="2"/>
+        <tr r="D24" s="2"/>
+        <tr r="D22" s="2"/>
+        <tr r="P21" s="2"/>
+        <tr r="H22" s="2"/>
+        <tr r="G25" s="2"/>
+        <tr r="I25" s="2"/>
+        <tr r="O19" s="2"/>
+        <tr r="J22" s="2"/>
+        <tr r="AA27" s="2"/>
+        <tr r="V20" s="2"/>
+        <tr r="C24" s="2"/>
+        <tr r="Q25" s="2"/>
+        <tr r="Z23" s="2"/>
+        <tr r="U22" s="2"/>
+        <tr r="C16" s="2"/>
+        <tr r="Q21" s="2"/>
+        <tr r="W22" s="2"/>
+        <tr r="H17" s="2"/>
+        <tr r="D18" s="2"/>
+        <tr r="M17" s="2"/>
+        <tr r="H18" s="2"/>
+        <tr r="N23" s="2"/>
+        <tr r="G22" s="2"/>
+        <tr r="T24" s="2"/>
+        <tr r="M16" s="2"/>
+        <tr r="L26" s="2"/>
+        <tr r="AA17" s="2"/>
+        <tr r="L21" s="2"/>
+        <tr r="D21" s="2"/>
+        <tr r="D25" s="2"/>
+        <tr r="C20" s="2"/>
+        <tr r="T26" s="2"/>
+        <tr r="AA25" s="2"/>
+        <tr r="X18" s="2"/>
+        <tr r="W27" s="2"/>
+        <tr r="G18" s="2"/>
+        <tr r="X25" s="2"/>
+        <tr r="X22" s="2"/>
+        <tr r="F17" s="2"/>
+        <tr r="M19" s="2"/>
+        <tr r="S22" s="2"/>
+        <tr r="W26" s="2"/>
+        <tr r="I27" s="2"/>
+        <tr r="O26" s="2"/>
+        <tr r="Z19" s="2"/>
+        <tr r="J19" s="2"/>
+        <tr r="X20" s="2"/>
+        <tr r="Y25" s="2"/>
+        <tr r="G20" s="2"/>
+        <tr r="S20" s="2"/>
+        <tr r="E27" s="2"/>
+        <tr r="J21" s="2"/>
+        <tr r="H19" s="2"/>
+        <tr r="K25" s="2"/>
+        <tr r="Z21" s="2"/>
+        <tr r="Z26" s="2"/>
+        <tr r="T19" s="2"/>
+        <tr r="X21" s="2"/>
+        <tr r="K23" s="2"/>
+        <tr r="E22" s="2"/>
+        <tr r="W18" s="2"/>
+        <tr r="X27" s="2"/>
+        <tr r="H23" s="2"/>
+        <tr r="P19" s="2"/>
+        <tr r="AA19" s="2"/>
+        <tr r="J17" s="2"/>
+        <tr r="U17" s="2"/>
+        <tr r="Q19" s="2"/>
+        <tr r="E16" s="2"/>
+        <tr r="G16" s="2"/>
+        <tr r="I16" s="2"/>
+        <tr r="W21" s="2"/>
+        <tr r="G21" s="2"/>
+        <tr r="Q24" s="2"/>
+        <tr r="F18" s="2"/>
+        <tr r="Z16" s="2"/>
+        <tr r="V25" s="2"/>
+        <tr r="X16" s="2"/>
+        <tr r="G24" s="2"/>
+        <tr r="N20" s="2"/>
+        <tr r="W25" s="2"/>
+        <tr r="R21" s="2"/>
+        <tr r="T16" s="2"/>
+        <tr r="O23" s="2"/>
+        <tr r="F27" s="2"/>
+        <tr r="U24" s="2"/>
+        <tr r="H24" s="2"/>
+        <tr r="C17" s="2"/>
+        <tr r="R22" s="2"/>
+        <tr r="N24" s="2"/>
+        <tr r="L25" s="2"/>
+        <tr r="H27" s="2"/>
+        <tr r="T22" s="2"/>
+        <tr r="D20" s="2"/>
+        <tr r="M20" s="2"/>
+        <tr r="P18" s="2"/>
+        <tr r="N21" s="2"/>
+        <tr r="D23" s="2"/>
+        <tr r="M22" s="2"/>
+        <tr r="C26" s="2"/>
+        <tr r="F16" s="2"/>
+        <tr r="S17" s="2"/>
+        <tr r="P23" s="2"/>
+        <tr r="AA26" s="2"/>
+        <tr r="N27" s="2"/>
+        <tr r="H20" s="2"/>
+        <tr r="D16" s="2"/>
+        <tr r="Z22" s="2"/>
+        <tr r="Z17" s="2"/>
+        <tr r="Y27" s="2"/>
+        <tr r="O18" s="2"/>
+        <tr r="K16" s="2"/>
+        <tr r="K20" s="2"/>
+        <tr r="I23" s="2"/>
+        <tr r="R20" s="2"/>
         <tr r="X24" s="2"/>
         <tr r="H26" s="2"/>
-        <tr r="U17" s="2"/>
-        <tr r="H17" s="2"/>
-        <tr r="O26" s="2"/>
-        <tr r="I16" s="2"/>
-        <tr r="N21" s="2"/>
+        <tr r="L18" s="2"/>
+        <tr r="G27" s="2"/>
+        <tr r="G17" s="2"/>
+        <tr r="K24" s="2"/>
+        <tr r="AA23" s="2"/>
+        <tr r="O22" s="2"/>
+        <tr r="F25" s="2"/>
+        <tr r="AA16" s="2"/>
+        <tr r="R23" s="2"/>
+        <tr r="S23" s="2"/>
+        <tr r="C18" s="2"/>
+        <tr r="N25" s="2"/>
+        <tr r="M27" s="2"/>
+        <tr r="G19" s="2"/>
+        <tr r="Q26" s="2"/>
+        <tr r="I21" s="2"/>
+        <tr r="T18" s="2"/>
+        <tr r="I24" s="2"/>
+        <tr r="Q23" s="2"/>
+        <tr r="V18" s="2"/>
+        <tr r="Y19" s="2"/>
+        <tr r="I20" s="2"/>
+        <tr r="C21" s="2"/>
+        <tr r="R18" s="2"/>
+        <tr r="Q16" s="2"/>
+        <tr r="N16" s="2"/>
+        <tr r="Q27" s="2"/>
+        <tr r="F24" s="2"/>
+        <tr r="N18" s="2"/>
+        <tr r="S26" s="2"/>
+        <tr r="O25" s="2"/>
+        <tr r="Z18" s="2"/>
+        <tr r="I22" s="2"/>
+        <tr r="F23" s="2"/>
+        <tr r="L24" s="2"/>
+        <tr r="K27" s="2"/>
         <tr r="T20" s="2"/>
-        <tr r="T18" s="2"/>
+        <tr r="U16" s="2"/>
+        <tr r="N19" s="2"/>
         <tr r="Q20" s="2"/>
+        <tr r="U23" s="2"/>
+        <tr r="P17" s="2"/>
+        <tr r="V16" s="2"/>
+        <tr r="F21" s="2"/>
+        <tr r="U27" s="2"/>
+        <tr r="U26" s="2"/>
+        <tr r="X19" s="2"/>
+        <tr r="R19" s="2"/>
+        <tr r="L20" s="2"/>
+        <tr r="K17" s="2"/>
+        <tr r="T21" s="2"/>
+        <tr r="V27" s="2"/>
+        <tr r="Y18" s="2"/>
+        <tr r="E24" s="2"/>
+        <tr r="Y23" s="2"/>
+        <tr r="M26" s="2"/>
+        <tr r="C25" s="2"/>
+        <tr r="R25" s="2"/>
+        <tr r="J16" s="2"/>
+        <tr r="K26" s="2"/>
+        <tr r="J24" s="2"/>
+        <tr r="J23" s="2"/>
+        <tr r="T25" s="2"/>
+        <tr r="G23" s="2"/>
         <tr r="N22" s="2"/>
-        <tr r="T23" s="2"/>
-        <tr r="Z24" s="2"/>
-        <tr r="M21" s="2"/>
-        <tr r="Q22" s="2"/>
-        <tr r="E23" s="2"/>
-        <tr r="O19" s="2"/>
-        <tr r="P19" s="2"/>
-        <tr r="D20" s="2"/>
-        <tr r="D18" s="2"/>
-        <tr r="Z19" s="2"/>
-        <tr r="W21" s="2"/>
-        <tr r="D23" s="2"/>
-        <tr r="J24" s="2"/>
-        <tr r="I24" s="2"/>
-        <tr r="U23" s="2"/>
         <tr r="Y16" s="2"/>
-        <tr r="L16" s="2"/>
-        <tr r="K22" s="2"/>
-        <tr r="J25" s="2"/>
-        <tr r="V22" s="2"/>
-        <tr r="H25" s="2"/>
-        <tr r="E17" s="2"/>
-        <tr r="AA16" s="2"/>
-        <tr r="M19" s="2"/>
-        <tr r="M17" s="2"/>
-        <tr r="J19" s="2"/>
-        <tr r="G21" s="2"/>
-        <tr r="M22" s="2"/>
-        <tr r="S23" s="2"/>
-        <tr r="Q23" s="2"/>
-        <tr r="P17" s="2"/>
         <tr r="V19" s="2"/>
-        <tr r="L23" s="2"/>
-        <tr r="D26" s="2"/>
-        <tr r="J20" s="2"/>
-        <tr r="D19" s="2"/>
-        <tr r="W23" s="2"/>
-        <tr r="F25" s="2"/>
-        <tr r="L25" s="2"/>
-        <tr r="C24" s="2"/>
-        <tr r="H18" s="2"/>
-        <tr r="X20" s="2"/>
-        <tr r="Q24" s="2"/>
-        <tr r="C26" s="2"/>
-        <tr r="G27" s="2"/>
-        <tr r="V18" s="2"/>
-        <tr r="V16" s="2"/>
         <tr r="S18" s="2"/>
-        <tr r="P20" s="2"/>
-        <tr r="V21" s="2"/>
-        <tr r="C23" s="2"/>
-        <tr r="Z25" s="2"/>
-        <tr r="J18" s="2"/>
-        <tr r="X25" s="2"/>
-        <tr r="J22" s="2"/>
-        <tr r="Q19" s="2"/>
-        <tr r="N23" s="2"/>
-        <tr r="Y25" s="2"/>
-        <tr r="F18" s="2"/>
-        <tr r="F16" s="2"/>
-        <tr r="C18" s="2"/>
-        <tr r="Y19" s="2"/>
-        <tr r="F21" s="2"/>
         <tr r="L22" s="2"/>
-        <tr r="V24" s="2"/>
-        <tr r="X23" s="2"/>
-        <tr r="K19" s="2"/>
-        <tr r="M18" s="2"/>
-        <tr r="W16" s="2"/>
-        <tr r="H23" s="2"/>
-        <tr r="X22" s="2"/>
-        <tr r="M20" s="2"/>
-        <tr r="G22" s="2"/>
-        <tr r="G20" s="2"/>
-        <tr r="Z16" s="2"/>
-        <tr r="S17" s="2"/>
-        <tr r="J23" s="2"/>
-        <tr r="I20" s="2"/>
-        <tr r="U27" s="2"/>
         <tr r="O17" s="2"/>
-        <tr r="R27" s="2"/>
-        <tr r="L17" s="2"/>
-        <tr r="I19" s="2"/>
-        <tr r="O20" s="2"/>
-        <tr r="U21" s="2"/>
-        <tr r="H22" s="2"/>
-        <tr r="AA19" s="2"/>
-        <tr r="Q25" s="2"/>
-        <tr r="T24" s="2"/>
-        <tr r="S20" s="2"/>
-        <tr r="V25" s="2"/>
-        <tr r="P23" s="2"/>
-        <tr r="G17" s="2"/>
-        <tr r="C21" s="2"/>
-        <tr r="U26" s="2"/>
         <tr r="W17" s="2"/>
-        <tr r="S27" s="2"/>
-        <tr r="D27" s="2"/>
-        <tr r="F19" s="2"/>
-        <tr r="Y20" s="2"/>
-        <tr r="I18" s="2"/>
-        <tr r="J16" s="2"/>
-        <tr r="H27" s="2"/>
-        <tr r="S22" s="2"/>
-        <tr r="M16" s="2"/>
-        <tr r="E27" s="2"/>
-        <tr r="X16" s="2"/>
-        <tr r="AA26" s="2"/>
-        <tr r="U16" s="2"/>
-        <tr r="R18" s="2"/>
-        <tr r="X19" s="2"/>
         <tr r="E21" s="2"/>
-        <tr r="E18" s="2"/>
-        <tr r="AA21" s="2"/>
-        <tr r="W24" s="2"/>
-        <tr r="D17" s="2"/>
-        <tr r="F20" s="2"/>
-        <tr r="N24" s="2"/>
-        <tr r="AA27" s="2"/>
-        <tr r="Z23" s="2"/>
-        <tr r="L26" s="2"/>
-        <tr r="J21" s="2"/>
-        <tr r="G24" s="2"/>
-        <tr r="N27" s="2"/>
-        <tr r="N25" s="2"/>
-        <tr r="Q16" s="2"/>
-        <tr r="R19" s="2"/>
         <tr r="R17" s="2"/>
-        <tr r="S19" s="2"/>
-        <tr r="S24" s="2"/>
-        <tr r="C22" s="2"/>
-        <tr r="R26" s="2"/>
-        <tr r="N26" s="2"/>
-        <tr r="H16" s="2"/>
-        <tr r="K26" s="2"/>
-        <tr r="E16" s="2"/>
-        <tr r="AA17" s="2"/>
-        <tr r="H19" s="2"/>
-        <tr r="N20" s="2"/>
-        <tr r="H20" s="2"/>
-        <tr r="K24" s="2"/>
-        <tr r="N16" s="2"/>
-        <tr r="L20" s="2"/>
         <tr r="E26" s="2"/>
-        <tr r="T27" s="2"/>
-        <tr r="X17" s="2"/>
-        <tr r="V17" s="2"/>
-        <tr r="V26" s="2"/>
-        <tr r="K18" s="2"/>
-        <tr r="P26" s="2"/>
-        <tr r="L18" s="2"/>
-        <tr r="U22" s="2"/>
-        <tr r="L21" s="2"/>
-        <tr r="K25" s="2"/>
-        <tr r="W25" s="2"/>
-        <tr r="D16" s="2"/>
-        <tr r="T25" s="2"/>
-        <tr r="Q27" s="2"/>
-        <tr r="K17" s="2"/>
         <tr r="Q18" s="2"/>
-        <tr r="W19" s="2"/>
-        <tr r="Y24" s="2"/>
-        <tr r="AA18" s="2"/>
-        <tr r="S21" s="2"/>
-        <tr r="H21" s="2"/>
-        <tr r="L19" s="2"/>
-        <tr r="K27" s="2"/>
-        <tr r="W26" s="2"/>
-        <tr r="D21" s="2"/>
-        <tr r="Z21" s="2"/>
-        <tr r="R21" s="2"/>
-        <tr r="Z22" s="2"/>
-        <tr r="M27" s="2"/>
-        <tr r="F24" s="2"/>
-        <tr r="T21" s="2"/>
         <tr r="E25" s="2"/>
-        <tr r="T17" s="2"/>
-        <tr r="R24" s="2"/>
-        <tr r="Z27" s="2"/>
-        <tr r="W20" s="2"/>
-        <tr r="U20" s="2"/>
-        <tr r="M23" s="2"/>
-        <tr r="G25" s="2"/>
-        <tr r="C16" s="2"/>
-        <tr r="D25" s="2"/>
-        <tr r="Z26" s="2"/>
-        <tr r="T16" s="2"/>
-        <tr r="Z17" s="2"/>
-        <tr r="G19" s="2"/>
-        <tr r="N18" s="2"/>
-        <tr r="V27" s="2"/>
         <tr r="O24" s="2"/>
-        <tr r="K21" s="2"/>
-        <tr r="C19" s="2"/>
-        <tr r="Y22" s="2"/>
-        <tr r="J27" s="2"/>
-        <tr r="Q17" s="2"/>
-        <tr r="U18" s="2"/>
-        <tr r="R23" s="2"/>
-        <tr r="G16" s="2"/>
-        <tr r="C20" s="2"/>
-        <tr r="T19" s="2"/>
-        <tr r="O23" s="2"/>
-        <tr r="Y27" s="2"/>
-        <tr r="AA23" s="2"/>
-        <tr r="S26" s="2"/>
-        <tr r="Y18" s="2"/>
         <tr r="E20" s="2"/>
-        <tr r="O21" s="2"/>
-        <tr r="P24" s="2"/>
-        <tr r="P22" s="2"/>
-        <tr r="M24" s="2"/>
-        <tr r="J26" s="2"/>
-        <tr r="P27" s="2"/>
-        <tr r="J17" s="2"/>
-        <tr r="P18" s="2"/>
-        <tr r="T26" s="2"/>
-        <tr r="X21" s="2"/>
-        <tr r="F27" s="2"/>
-        <tr r="O18" s="2"/>
-        <tr r="Q26" s="2"/>
-        <tr r="O25" s="2"/>
-        <tr r="E24" s="2"/>
         <tr r="U25" s="2"/>
-        <tr r="O16" s="2"/>
-        <tr r="AA20" s="2"/>
-        <tr r="G26" s="2"/>
-        <tr r="Z20" s="2"/>
-        <tr r="N17" s="2"/>
-        <tr r="L27" s="2"/>
-        <tr r="F17" s="2"/>
-        <tr r="Q21" s="2"/>
-        <tr r="AA25" s="2"/>
-        <tr r="K23" s="2"/>
-        <tr r="U24" s="2"/>
-        <tr r="K16" s="2"/>
-        <tr r="N19" s="2"/>
-        <tr r="Z18" s="2"/>
-        <tr r="Y23" s="2"/>
         <tr r="Y21" s="2"/>
-        <tr r="V23" s="2"/>
-        <tr r="S25" s="2"/>
-        <tr r="Y26" s="2"/>
-        <tr r="S16" s="2"/>
-        <tr r="Y17" s="2"/>
-        <tr r="AA24" s="2"/>
-        <tr r="V20" s="2"/>
-        <tr r="I27" s="2"/>
-        <tr r="X18" s="2"/>
-        <tr r="E22" s="2"/>
-        <tr r="H24" s="2"/>
-        <tr r="K20" s="2"/>
-        <tr r="G23" s="2"/>
-        <tr r="I22" s="2"/>
-        <tr r="M26" s="2"/>
         <tr r="F26" s="2"/>
-        <tr r="AA22" s="2"/>
-        <tr r="U19" s="2"/>
-        <tr r="P25" s="2"/>
-        <tr r="C27" s="2"/>
-        <tr r="E19" s="2"/>
-        <tr r="D24" s="2"/>
-        <tr r="T22" s="2"/>
-        <tr r="W22" s="2"/>
-        <tr r="W27" s="2"/>
-        <tr r="W18" s="2"/>
-        <tr r="C17" s="2"/>
-        <tr r="I23" s="2"/>
-        <tr r="I21" s="2"/>
-        <tr r="F23" s="2"/>
-        <tr r="C25" s="2"/>
         <tr r="I26" s="2"/>
-        <tr r="O27" s="2"/>
-        <tr r="I17" s="2"/>
-        <tr r="M25" s="2"/>
-        <tr r="P16" s="2"/>
-        <tr r="F22" s="2"/>
-        <tr r="D22" s="2"/>
-        <tr r="P21" s="2"/>
-        <tr r="I25" s="2"/>
-        <tr r="G18" s="2"/>
-        <tr r="X27" s="2"/>
-        <tr r="R22" s="2"/>
-        <tr r="R20" s="2"/>
-        <tr r="O22" s="2"/>
-        <tr r="L24" s="2"/>
-        <tr r="R25" s="2"/>
         <tr r="X26" s="2"/>
         <tr r="R16" s="2"/>
       </tp>
     </main>
-    <main first="rtdsrv.18df948ffd4747e49d738fb50ed12bec">
+    <main first="rtdsrv.9ab47963834640bc914c733d5ccad4d8">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>a909e5ee-15c7-43e3-9ee8-aa5852c79f7b</stp>
+        <stp>ef729c81-1fef-416c-b027-efd040b8e69d</stp>
+        <tr r="J17" s="1"/>
+        <tr r="L17" s="1"/>
+        <tr r="F18" s="1"/>
+        <tr r="H22" s="1"/>
+        <tr r="D20" s="1"/>
+        <tr r="E22" s="1"/>
+        <tr r="H17" s="1"/>
+        <tr r="G25" s="1"/>
+        <tr r="I27" s="1"/>
+        <tr r="F27" s="1"/>
+        <tr r="G16" s="1"/>
+        <tr r="L23" s="1"/>
+        <tr r="Q26" s="1"/>
+        <tr r="E23" s="1"/>
+        <tr r="I24" s="1"/>
+        <tr r="J24" s="1"/>
+        <tr r="F19" s="1"/>
+        <tr r="L19" s="1"/>
+        <tr r="J19" s="1"/>
+        <tr r="G21" s="1"/>
+        <tr r="P18" s="1"/>
         <tr r="L22" s="1"/>
-        <tr r="F27" s="1"/>
+        <tr r="H26" s="1"/>
+        <tr r="K25" s="1"/>
+        <tr r="D25" s="1"/>
+        <tr r="F26" s="1"/>
         <tr r="M26" s="1"/>
+        <tr r="E20" s="1"/>
+        <tr r="J16" s="1"/>
+        <tr r="E19" s="1"/>
+        <tr r="L21" s="1"/>
+        <tr r="N17" s="1"/>
+        <tr r="G26" s="1"/>
+        <tr r="F21" s="1"/>
+        <tr r="E18" s="1"/>
+        <tr r="I18" s="1"/>
+        <tr r="O19" s="1"/>
+        <tr r="M19" s="1"/>
+        <tr r="L24" s="1"/>
+        <tr r="P19" s="1"/>
+        <tr r="I23" s="1"/>
+        <tr r="F25" s="1"/>
+        <tr r="L27" s="1"/>
+        <tr r="Q24" s="1"/>
+        <tr r="I19" s="1"/>
+        <tr r="F20" s="1"/>
+        <tr r="F24" s="1"/>
+        <tr r="H23" s="1"/>
+        <tr r="Q18" s="1"/>
+        <tr r="C16" s="1"/>
+        <tr r="C22" s="1"/>
         <tr r="C20" s="1"/>
+        <tr r="O23" s="1"/>
+        <tr r="D27" s="1"/>
+        <tr r="Q20" s="1"/>
+        <tr r="G20" s="1"/>
+        <tr r="E25" s="1"/>
+        <tr r="K20" s="1"/>
+        <tr r="D16" s="1"/>
+        <tr r="O26" s="1"/>
+        <tr r="O22" s="1"/>
+        <tr r="L16" s="1"/>
+        <tr r="E24" s="1"/>
+        <tr r="Q23" s="1"/>
+        <tr r="F22" s="1"/>
+        <tr r="P20" s="1"/>
+        <tr r="Q17" s="1"/>
+        <tr r="J18" s="1"/>
+        <tr r="H20" s="1"/>
+        <tr r="I20" s="1"/>
+        <tr r="D17" s="1"/>
+        <tr r="C24" s="1"/>
+        <tr r="O27" s="1"/>
+        <tr r="F23" s="1"/>
+        <tr r="C18" s="1"/>
+        <tr r="D19" s="1"/>
+        <tr r="M25" s="1"/>
+        <tr r="K27" s="1"/>
+        <tr r="E26" s="1"/>
+        <tr r="P16" s="1"/>
+        <tr r="K22" s="1"/>
+        <tr r="L20" s="1"/>
+        <tr r="K21" s="1"/>
+        <tr r="M20" s="1"/>
+        <tr r="O17" s="1"/>
+        <tr r="K18" s="1"/>
+        <tr r="P26" s="1"/>
+        <tr r="K23" s="1"/>
+        <tr r="N26" s="1"/>
+        <tr r="C26" s="1"/>
+        <tr r="J25" s="1"/>
+        <tr r="F17" s="1"/>
+        <tr r="H25" s="1"/>
+        <tr r="D24" s="1"/>
+        <tr r="D21" s="1"/>
+        <tr r="O20" s="1"/>
+        <tr r="O21" s="1"/>
+        <tr r="M21" s="1"/>
+        <tr r="M17" s="1"/>
+        <tr r="K19" s="1"/>
+        <tr r="P23" s="1"/>
+        <tr r="N19" s="1"/>
+        <tr r="E27" s="1"/>
+        <tr r="J22" s="1"/>
+        <tr r="L26" s="1"/>
+        <tr r="Q27" s="1"/>
+        <tr r="P24" s="1"/>
+        <tr r="C23" s="1"/>
+        <tr r="C19" s="1"/>
+        <tr r="G17" s="1"/>
+        <tr r="Q25" s="1"/>
+        <tr r="N18" s="1"/>
+        <tr r="O24" s="1"/>
+        <tr r="H18" s="1"/>
+        <tr r="H27" s="1"/>
+        <tr r="M24" s="1"/>
+        <tr r="D18" s="1"/>
+        <tr r="Q22" s="1"/>
+        <tr r="H16" s="1"/>
+        <tr r="M22" s="1"/>
+        <tr r="D23" s="1"/>
+        <tr r="C21" s="1"/>
+        <tr r="G22" s="1"/>
+        <tr r="H21" s="1"/>
+        <tr r="C25" s="1"/>
+        <tr r="L18" s="1"/>
+        <tr r="J26" s="1"/>
+        <tr r="I17" s="1"/>
+        <tr r="Q21" s="1"/>
+        <tr r="O25" s="1"/>
+        <tr r="I25" s="1"/>
+        <tr r="J21" s="1"/>
+        <tr r="M16" s="1"/>
+        <tr r="I16" s="1"/>
+        <tr r="P22" s="1"/>
+        <tr r="H24" s="1"/>
+        <tr r="G27" s="1"/>
+        <tr r="J20" s="1"/>
+        <tr r="D22" s="1"/>
+        <tr r="K17" s="1"/>
+        <tr r="G24" s="1"/>
+        <tr r="N25" s="1"/>
+        <tr r="K26" s="1"/>
+        <tr r="K16" s="1"/>
+        <tr r="K24" s="1"/>
+        <tr r="I21" s="1"/>
+        <tr r="Q19" s="1"/>
+        <tr r="N16" s="1"/>
+        <tr r="P25" s="1"/>
+        <tr r="I26" s="1"/>
+        <tr r="Q16" s="1"/>
+        <tr r="N23" s="1"/>
+        <tr r="D26" s="1"/>
+        <tr r="M27" s="1"/>
+        <tr r="N27" s="1"/>
+        <tr r="F16" s="1"/>
+        <tr r="O18" s="1"/>
+        <tr r="C17" s="1"/>
+        <tr r="E17" s="1"/>
+        <tr r="J27" s="1"/>
+        <tr r="P17" s="1"/>
         <tr r="M18" s="1"/>
-        <tr r="K20" s="1"/>
-        <tr r="J25" s="1"/>
-        <tr r="E24" s="1"/>
-        <tr r="Q25" s="1"/>
-        <tr r="O20" s="1"/>
-        <tr r="O24" s="1"/>
+        <tr r="L25" s="1"/>
         <tr r="P27" s="1"/>
-        <tr r="H24" s="1"/>
-        <tr r="D26" s="1"/>
+        <tr r="M23" s="1"/>
+        <tr r="N21" s="1"/>
+        <tr r="N22" s="1"/>
+        <tr r="H19" s="1"/>
+        <tr r="E21" s="1"/>
         <tr r="I22" s="1"/>
-        <tr r="P17" s="1"/>
-        <tr r="L17" s="1"/>
-        <tr r="G16" s="1"/>
-        <tr r="E20" s="1"/>
-        <tr r="P19" s="1"/>
-        <tr r="P24" s="1"/>
-        <tr r="D19" s="1"/>
-        <tr r="K27" s="1"/>
-        <tr r="Q23" s="1"/>
-        <tr r="K22" s="1"/>
-        <tr r="O21" s="1"/>
-        <tr r="H18" s="1"/>
-        <tr r="J26" s="1"/>
-        <tr r="G27" s="1"/>
-        <tr r="N22" s="1"/>
         <tr r="C27" s="1"/>
-        <tr r="O23" s="1"/>
-        <tr r="E22" s="1"/>
-        <tr r="L23" s="1"/>
-        <tr r="J16" s="1"/>
-        <tr r="I23" s="1"/>
-        <tr r="N16" s="1"/>
-        <tr r="L18" s="1"/>
-        <tr r="O26" s="1"/>
-        <tr r="F22" s="1"/>
-        <tr r="D24" s="1"/>
-        <tr r="M21" s="1"/>
-        <tr r="H27" s="1"/>
-        <tr r="Q16" s="1"/>
-        <tr r="J20" s="1"/>
-        <tr r="M27" s="1"/>
         <tr r="O16" s="1"/>
-        <tr r="K23" s="1"/>
-        <tr r="H26" s="1"/>
-        <tr r="Q26" s="1"/>
-        <tr r="E19" s="1"/>
-        <tr r="F25" s="1"/>
-        <tr r="D27" s="1"/>
-        <tr r="J21" s="1"/>
-        <tr r="C19" s="1"/>
-        <tr r="P20" s="1"/>
-        <tr r="L20" s="1"/>
-        <tr r="M17" s="1"/>
-        <tr r="M24" s="1"/>
-        <tr r="M16" s="1"/>
-        <tr r="D22" s="1"/>
-        <tr r="H19" s="1"/>
         <tr r="G18" s="1"/>
-        <tr r="L24" s="1"/>
-        <tr r="F18" s="1"/>
-        <tr r="E23" s="1"/>
-        <tr r="L21" s="1"/>
-        <tr r="L27" s="1"/>
-        <tr r="C22" s="1"/>
-        <tr r="C26" s="1"/>
-        <tr r="F17" s="1"/>
-        <tr r="Q17" s="1"/>
-        <tr r="N18" s="1"/>
-        <tr r="K19" s="1"/>
-        <tr r="D18" s="1"/>
-        <tr r="M23" s="1"/>
-        <tr r="K17" s="1"/>
-        <tr r="N27" s="1"/>
         <tr r="J23" s="1"/>
-        <tr r="Q19" s="1"/>
-        <tr r="H17" s="1"/>
-        <tr r="I24" s="1"/>
-        <tr r="N17" s="1"/>
-        <tr r="Q24" s="1"/>
-        <tr r="N26" s="1"/>
-        <tr r="I26" s="1"/>
-        <tr r="E26" s="1"/>
-        <tr r="J18" s="1"/>
-        <tr r="K21" s="1"/>
-        <tr r="P23" s="1"/>
-        <tr r="Q22" s="1"/>
-        <tr r="I17" s="1"/>
-        <tr r="G24" s="1"/>
-        <tr r="E21" s="1"/>
         <tr r="N24" s="1"/>
-        <tr r="F23" s="1"/>
-        <tr r="K25" s="1"/>
-        <tr r="J24" s="1"/>
-        <tr r="G26" s="1"/>
-        <tr r="I19" s="1"/>
-        <tr r="C18" s="1"/>
-        <tr r="C23" s="1"/>
-        <tr r="O22" s="1"/>
-        <tr r="H20" s="1"/>
-        <tr r="D21" s="1"/>
-        <tr r="N19" s="1"/>
-        <tr r="H16" s="1"/>
-        <tr r="I16" s="1"/>
-        <tr r="N25" s="1"/>
-        <tr r="F16" s="1"/>
         <tr r="G19" s="1"/>
-        <tr r="O25" s="1"/>
-        <tr r="G25" s="1"/>
-        <tr r="F19" s="1"/>
-        <tr r="F21" s="1"/>
-        <tr r="F20" s="1"/>
-        <tr r="I25" s="1"/>
-        <tr r="L25" s="1"/>
-        <tr r="H25" s="1"/>
-        <tr r="I20" s="1"/>
-        <tr r="M20" s="1"/>
-        <tr r="E27" s="1"/>
-        <tr r="M22" s="1"/>
-        <tr r="N23" s="1"/>
-        <tr r="K26" s="1"/>
-        <tr r="O18" s="1"/>
         <tr r="E16" s="1"/>
-        <tr r="D20" s="1"/>
-        <tr r="D25" s="1"/>
-        <tr r="L19" s="1"/>
-        <tr r="E18" s="1"/>
-        <tr r="F24" s="1"/>
-        <tr r="C25" s="1"/>
-        <tr r="D16" s="1"/>
-        <tr r="G17" s="1"/>
-        <tr r="D17" s="1"/>
-        <tr r="O17" s="1"/>
-        <tr r="J22" s="1"/>
-        <tr r="D23" s="1"/>
-        <tr r="N21" s="1"/>
-        <tr r="K16" s="1"/>
-        <tr r="C17" s="1"/>
         <tr r="G23" s="1"/>
-        <tr r="H21" s="1"/>
-        <tr r="I27" s="1"/>
-        <tr r="J19" s="1"/>
-        <tr r="I18" s="1"/>
-        <tr r="H23" s="1"/>
-        <tr r="E25" s="1"/>
-        <tr r="M25" s="1"/>
-        <tr r="P16" s="1"/>
-        <tr r="C24" s="1"/>
-        <tr r="K18" s="1"/>
-        <tr r="L26" s="1"/>
-        <tr r="C21" s="1"/>
-        <tr r="P22" s="1"/>
-        <tr r="K24" s="1"/>
-        <tr r="E17" s="1"/>
         <tr r="N20" s="1"/>
-        <tr r="G20" s="1"/>
-        <tr r="F26" s="1"/>
-        <tr r="G21" s="1"/>
-        <tr r="O19" s="1"/>
-        <tr r="Q18" s="1"/>
-        <tr r="P25" s="1"/>
-        <tr r="Q20" s="1"/>
-        <tr r="L16" s="1"/>
-        <tr r="O27" s="1"/>
-        <tr r="P26" s="1"/>
-        <tr r="Q27" s="1"/>
-        <tr r="G22" s="1"/>
-        <tr r="Q21" s="1"/>
-        <tr r="I21" s="1"/>
-        <tr r="J27" s="1"/>
         <tr r="P21" s="1"/>
-        <tr r="J17" s="1"/>
-        <tr r="H22" s="1"/>
-        <tr r="P18" s="1"/>
-        <tr r="M19" s="1"/>
-        <tr r="C16" s="1"/>
       </tp>
     </main>
   </volType>
@@ -1155,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F32773-32F6-4E82-8FD8-8EE0575AC374}">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1398,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5"/>
@@ -1471,7 +1456,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="5"/>
@@ -1529,7 +1514,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5"/>
@@ -1654,13 +1639,13 @@
         <v>Instrument Ids</v>
       </c>
       <c r="O16" s="6" t="str">
-        <v>LookThroughPortfolioId Scope</v>
-      </c>
-      <c r="P16" s="7" t="str">
-        <v>LookThroughPortfolioId Code</v>
-      </c>
-      <c r="Q16" s="6" t="str">
         <v>Name</v>
+      </c>
+      <c r="P16" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q16" s="1" t="str">
+        <v/>
       </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1675,50 +1660,50 @@
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>43790</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>43972</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>100000000</v>
       </c>
-      <c r="F17" s="8" t="str">
+      <c r="F17" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>-128863000</v>
       </c>
-      <c r="H17" s="8" t="str">
+      <c r="H17" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="7">
         <v>1.2886299999999999</v>
       </c>
-      <c r="J17" s="8" t="b">
+      <c r="J17" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="7">
         <v>43790</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="7">
         <v>0</v>
       </c>
-      <c r="M17" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N17" s="8" t="str">
-        <v>LUID_2W533GOV,FXFWD0001</v>
-      </c>
-      <c r="O17" s="8">
-        <v>0</v>
-      </c>
-      <c r="P17" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="8" t="str">
-        <v>FXFWD1-Update</v>
+      <c r="M17" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N17" s="7" t="str">
+        <v>FXFWD0001,LUID_2W533GOV</v>
+      </c>
+      <c r="O17" s="7" t="str">
+        <v>FXFWD1-UpdateTheSecond</v>
+      </c>
+      <c r="P17" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q17" s="1" t="str">
+        <v/>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -1733,50 +1718,50 @@
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>43790</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>43972</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>50000000</v>
       </c>
-      <c r="F18" s="8" t="str">
+      <c r="F18" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>-64431500</v>
       </c>
-      <c r="H18" s="8" t="str">
+      <c r="H18" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <v>1.2886299999999999</v>
       </c>
-      <c r="J18" s="8" t="b">
+      <c r="J18" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="7">
         <v>43790</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="7">
         <v>0</v>
       </c>
-      <c r="M18" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N18" s="8" t="str">
-        <v>LUID_1UDR6T2I,FXFWD0002</v>
-      </c>
-      <c r="O18" s="8">
-        <v>0</v>
-      </c>
-      <c r="P18" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="8" t="str">
+      <c r="M18" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N18" s="7" t="str">
+        <v>FXFWD0002,LUID_1UDR6T2I</v>
+      </c>
+      <c r="O18" s="7" t="str">
         <v>FXFWD2</v>
+      </c>
+      <c r="P18" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q18" s="1" t="str">
+        <v/>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1791,50 +1776,50 @@
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>43957.684771770837</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <v>44322.684771770837</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>1</v>
       </c>
-      <c r="F19" s="8" t="str">
+      <c r="F19" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>-1.3</v>
       </c>
-      <c r="H19" s="8" t="str">
+      <c r="H19" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="7">
         <v>1</v>
       </c>
-      <c r="J19" s="8" t="b">
+      <c r="J19" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="7">
         <v>43957.684771770837</v>
       </c>
-      <c r="L19" s="8">
+      <c r="L19" s="7">
         <v>0</v>
       </c>
-      <c r="M19" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N19" s="8" t="str">
-        <v>LUID_F0UY3CY8,FxForward-637243791205499396</v>
-      </c>
-      <c r="O19" s="8">
-        <v>0</v>
-      </c>
-      <c r="P19" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="8" t="str">
+      <c r="M19" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N19" s="7" t="str">
+        <v>FxForward-637243791205499396,LUID_F0UY3CY8</v>
+      </c>
+      <c r="O19" s="7" t="str">
         <v>FxForward-637243791205499396</v>
+      </c>
+      <c r="P19" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q19" s="1" t="str">
+        <v/>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -1849,50 +1834,50 @@
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>43983</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>43990</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>1</v>
       </c>
-      <c r="F20" s="8" t="str">
+      <c r="F20" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>-1.2508999999999999</v>
       </c>
-      <c r="H20" s="8" t="str">
+      <c r="H20" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="7">
         <v>1.2507999999999999</v>
       </c>
-      <c r="J20" s="8" t="b">
+      <c r="J20" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="7">
         <v>0</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="7">
         <v>0</v>
       </c>
-      <c r="M20" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N20" s="8" t="str">
-        <v>LUID_JW6AVI4S,gbp_usd_fwd_1w_12509</v>
-      </c>
-      <c r="O20" s="8">
-        <v>0</v>
-      </c>
-      <c r="P20" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="8" t="str">
+      <c r="M20" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N20" s="7" t="str">
+        <v>gbp_usd_fwd_1w_12509,LUID_JW6AVI4S</v>
+      </c>
+      <c r="O20" s="7" t="str">
         <v>GBP/USD 1W @ 1.2509</v>
+      </c>
+      <c r="P20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q20" s="1" t="str">
+        <v/>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -1907,50 +1892,50 @@
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>43868</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>44092</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>1</v>
       </c>
-      <c r="F21" s="8" t="str">
+      <c r="F21" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>-123</v>
       </c>
-      <c r="H21" s="8" t="str">
+      <c r="H21" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="7">
         <v>100</v>
       </c>
-      <c r="J21" s="8" t="b">
+      <c r="J21" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="7">
         <v>44061</v>
       </c>
-      <c r="L21" s="8">
+      <c r="L21" s="7">
         <v>0</v>
       </c>
-      <c r="M21" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N21" s="8" t="str">
-        <v>LUID_XHV68ZZA,FxForward_uniqueId</v>
-      </c>
-      <c r="O21" s="8">
-        <v>0</v>
-      </c>
-      <c r="P21" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="8" t="str">
+      <c r="M21" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N21" s="7" t="str">
+        <v>FxForward_uniqueId,LUID_XHV68ZZA</v>
+      </c>
+      <c r="O21" s="7" t="str">
         <v>FxForward</v>
+      </c>
+      <c r="P21" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q21" s="1" t="str">
+        <v/>
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -1965,50 +1950,50 @@
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>44512</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <v>44608</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <v>-1000000</v>
       </c>
-      <c r="F22" s="8" t="str">
+      <c r="F22" s="7" t="str">
         <v>EUR</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>1147777</v>
       </c>
-      <c r="H22" s="8" t="str">
+      <c r="H22" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="7">
         <v>1.1448</v>
       </c>
-      <c r="J22" s="8" t="b">
+      <c r="J22" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K22" s="7">
         <v>44607</v>
       </c>
-      <c r="L22" s="8" t="str">
+      <c r="L22" s="7" t="str">
         <v>EUR</v>
       </c>
-      <c r="M22" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N22" s="8" t="str">
-        <v>LUID_T9IFXCOY,InterestRateSwap_uniqueId</v>
-      </c>
-      <c r="O22" s="8">
-        <v>0</v>
-      </c>
-      <c r="P22" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="8" t="str">
+      <c r="M22" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N22" s="7" t="str">
+        <v>InterestRateSwap_uniqueId,LUID_T9IFXCOY</v>
+      </c>
+      <c r="O22" s="7" t="str">
         <v>InterestRateSwap</v>
+      </c>
+      <c r="P22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q22" s="1" t="str">
+        <v/>
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2023,50 +2008,50 @@
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>43868</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>44092</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>-1</v>
       </c>
-      <c r="F23" s="8" t="str">
+      <c r="F23" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>109</v>
       </c>
-      <c r="H23" s="8" t="str">
+      <c r="H23" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="7">
         <v>0</v>
       </c>
-      <c r="J23" s="8" t="b">
+      <c r="J23" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K23" s="7">
         <v>0</v>
       </c>
-      <c r="L23" s="8">
+      <c r="L23" s="7">
         <v>0</v>
       </c>
-      <c r="M23" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N23" s="8" t="str">
-        <v>LUID_PS1AKQYM,id-fxfwd-2</v>
-      </c>
-      <c r="O23" s="8">
-        <v>0</v>
-      </c>
-      <c r="P23" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="8" t="str">
+      <c r="M23" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N23" s="7" t="str">
+        <v>id-fxfwd-2,LUID_PS1AKQYM</v>
+      </c>
+      <c r="O23" s="7" t="str">
         <v>some-name-for-this-fxforward</v>
+      </c>
+      <c r="P23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q23" s="1" t="str">
+        <v/>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -2081,50 +2066,50 @@
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>43868</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="7">
         <v>44092</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>-1</v>
       </c>
-      <c r="F24" s="8" t="str">
+      <c r="F24" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="7">
         <v>109</v>
       </c>
-      <c r="H24" s="8" t="str">
+      <c r="H24" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="7">
         <v>0</v>
       </c>
-      <c r="J24" s="8" t="b">
+      <c r="J24" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24" s="7">
         <v>0</v>
       </c>
-      <c r="L24" s="8">
+      <c r="L24" s="7">
         <v>0</v>
       </c>
-      <c r="M24" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N24" s="8" t="str">
-        <v>LUID_GM2M6MIJ,id-fxfwd-for-pricing</v>
-      </c>
-      <c r="O24" s="8">
-        <v>0</v>
-      </c>
-      <c r="P24" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="8" t="str">
+      <c r="M24" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N24" s="7" t="str">
+        <v>id-fxfwd-for-pricing,LUID_GM2M6MIJ</v>
+      </c>
+      <c r="O24" s="7" t="str">
         <v>some-name-for-this-fxforward</v>
+      </c>
+      <c r="P24" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q24" s="1" t="str">
+        <v/>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2139,50 +2124,50 @@
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>43868</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <v>44092</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <v>-1</v>
       </c>
-      <c r="F25" s="8" t="str">
+      <c r="F25" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="7">
         <v>109</v>
       </c>
-      <c r="H25" s="8" t="str">
+      <c r="H25" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="7">
         <v>0</v>
       </c>
-      <c r="J25" s="8" t="b">
+      <c r="J25" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="7">
         <v>0</v>
       </c>
-      <c r="L25" s="8">
+      <c r="L25" s="7">
         <v>0</v>
       </c>
-      <c r="M25" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N25" s="8" t="str">
-        <v>LUID_38KBBI2D,LUID_00001234</v>
-      </c>
-      <c r="O25" s="8">
-        <v>0</v>
-      </c>
-      <c r="P25" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="8" t="str">
+      <c r="M25" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N25" s="7" t="str">
+        <v>LUID_00001234,LUID_38KBBI2D</v>
+      </c>
+      <c r="O25" s="7" t="str">
         <v>some-name-for-this-fxforward</v>
+      </c>
+      <c r="P25" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q25" s="1" t="str">
+        <v/>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -2197,50 +2182,50 @@
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>44249</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <v>44614</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <v>-1</v>
       </c>
-      <c r="F26" s="8" t="str">
+      <c r="F26" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="7">
         <v>109</v>
       </c>
-      <c r="H26" s="8" t="str">
+      <c r="H26" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="7">
         <v>0</v>
       </c>
-      <c r="J26" s="8" t="b">
+      <c r="J26" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="7">
         <v>0</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L26" s="7">
         <v>0</v>
       </c>
-      <c r="M26" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N26" s="8" t="str">
-        <v>LUID_7KPMGPYY,usd-jpy-fwd</v>
-      </c>
-      <c r="O26" s="8">
-        <v>0</v>
-      </c>
-      <c r="P26" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="8" t="str">
+      <c r="M26" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N26" s="7" t="str">
+        <v>usd-jpy-fwd,LUID_7KPMGPYY</v>
+      </c>
+      <c r="O26" s="7" t="str">
         <v>some-name-for-this-fxforward</v>
+      </c>
+      <c r="P26" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q26" s="1" t="str">
+        <v/>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -2255,50 +2240,50 @@
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="8" t="str">
+      <c r="C27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="D27" s="8" t="str">
+      <c r="D27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="E27" s="8" t="str">
+      <c r="E27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="F27" s="8" t="str">
+      <c r="F27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="G27" s="8" t="str">
+      <c r="G27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="H27" s="8" t="str">
+      <c r="H27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="I27" s="8" t="str">
+      <c r="I27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="J27" s="8" t="str">
+      <c r="J27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="K27" s="8" t="str">
+      <c r="K27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="L27" s="8" t="str">
+      <c r="L27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="M27" s="8" t="str">
+      <c r="M27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="N27" s="8" t="str">
+      <c r="N27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="O27" s="8" t="str">
+      <c r="O27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="P27" s="9" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="Q27" s="8" t="str">
-        <v>[More...]</v>
+      <c r="P27" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q27" s="1" t="str">
+        <v/>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -2466,12 +2451,8 @@
       <c r="O32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P32" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
@@ -2485,21 +2466,21 @@
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="8"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
@@ -2513,21 +2494,21 @@
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="8"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
@@ -2541,21 +2522,21 @@
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="8"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
@@ -2569,21 +2550,21 @@
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
@@ -2597,21 +2578,21 @@
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
@@ -2625,21 +2606,21 @@
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="8"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
@@ -2653,21 +2634,21 @@
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="8"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
@@ -2681,21 +2662,21 @@
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -2709,21 +2690,21 @@
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
@@ -2795,22 +2776,22 @@
       <c r="Z43" s="1"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="15">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name" sqref="C32" xr:uid="{A1279EB5-614B-4394-8A00-AA32F2E4B821}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Types" sqref="D32" xr:uid="{325D66AF-547B-4A63-BB8B-F160312D5817}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Ids" sqref="E32" xr:uid="{E64BCE8B-D3AC-4268-BB94-ECF82351123D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LookThroughPortfolioId Scope" sqref="F32" xr:uid="{8107FBD1-8557-4D57-BBBB-70A05EDED1AF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LookThroughPortfolioId Code" sqref="G32" xr:uid="{33E90796-7E7D-4A8E-B27C-917BE0E62729}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="StartDate" sqref="H32" xr:uid="{50D2ED42-56E6-409C-9BC4-E44C6CB6AA7F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="MaturityDate" sqref="I32" xr:uid="{791152C1-866D-4FB2-8683-7D0DEECDC9C3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DomAmount" sqref="J32" xr:uid="{88E0C8A9-373B-4E98-98C2-AB6A5B49B7E3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DomCcy" sqref="K32" xr:uid="{64634901-DC08-4F72-B640-CEC1CE520FA5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FgnAmount" sqref="L32" xr:uid="{2348A54C-FE34-49EE-BFE1-029A826E4793}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FgnCcy" sqref="M32" xr:uid="{9213113A-0398-4FC0-A559-8D3F55FD1A74}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="RefSpotRate" sqref="N32" xr:uid="{CC32103D-1FEF-450D-AF76-C58E5441330E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="IsNdf" sqref="O32" xr:uid="{9119B468-A600-4DB3-903F-7E9E878B0981}"/>
+  <dataValidations count="15">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FixingDate" sqref="P32" xr:uid="{2F2105F9-068C-47FC-9681-F303D0090D1B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="SettlementCcy" sqref="Q32" xr:uid="{5F4C1BCF-1DAE-407F-B62A-5CE1C6997A92}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name" sqref="C32" xr:uid="{BD61CCDD-5CE1-491E-8D11-69DB5C10779F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Types" sqref="D32" xr:uid="{DEEAC682-59C8-429D-9278-7A76298A1D8B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Ids" sqref="E32" xr:uid="{A02F9862-D4BE-4BC5-BCD2-DC184AEB5BF3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="StartDate" sqref="F32" xr:uid="{7E337B47-A352-420A-B3BF-3E2195A09566}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="MaturityDate" sqref="G32" xr:uid="{9A946B9C-D7CC-42ED-A3F8-02B651C06B02}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DomAmount" sqref="H32" xr:uid="{52DF61F3-24BB-40C7-997A-B038EBAED45E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DomCcy" sqref="I32" xr:uid="{4D45BB1D-DF51-405B-9C16-B47D030CCC23}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FgnAmount" sqref="J32" xr:uid="{15480889-C640-4900-B79A-0BCD963F567D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FgnCcy" sqref="K32" xr:uid="{7993F5F2-7963-4DE8-9EA3-0A2941463547}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="RefSpotRate" sqref="L32" xr:uid="{F569D225-F547-446D-8CEF-B734782E6173}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="IsNdf" sqref="M32" xr:uid="{7EF8A577-5C0E-4E71-9193-4B65F9883336}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FixingDate" sqref="N32" xr:uid="{C2B159A6-C107-4770-9AF6-8289B17C4024}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="SettlementCcy" sqref="O32" xr:uid="{31D8D0B2-A37A-43C7-BF00-F6D22D3E9644}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2820,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90759B6D-4CB9-4D5B-BC0B-C7D05AD9C258}">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2920,7 +2901,7 @@
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2953,7 +2934,7 @@
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3048,7 +3029,7 @@
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -3111,7 +3092,7 @@
     </row>
     <row r="9" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5"/>
@@ -3175,7 +3156,7 @@
     </row>
     <row r="11" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="5"/>
@@ -3239,7 +3220,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5"/>
@@ -3403,13 +3384,13 @@
         <v>Instrument Ids</v>
       </c>
       <c r="Y16" s="6" t="str">
-        <v>LookThroughPortfolioId Scope</v>
-      </c>
-      <c r="Z16" s="6" t="str">
-        <v>LookThroughPortfolioId Code</v>
-      </c>
-      <c r="AA16" s="6" t="str">
         <v>Name</v>
+      </c>
+      <c r="Z16" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA16" s="1" t="str">
+        <v/>
       </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
@@ -3417,80 +3398,80 @@
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>43835</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>43866</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>1000000</v>
       </c>
-      <c r="F17" s="8" t="str">
+      <c r="F17" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>-1380000</v>
       </c>
-      <c r="H17" s="8" t="str">
+      <c r="H17" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="7">
         <v>1.38</v>
       </c>
-      <c r="J17" s="8" t="b">
+      <c r="J17" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="7">
         <v>43835</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="7">
         <v>0</v>
       </c>
-      <c r="M17" s="8">
+      <c r="M17" s="7">
         <v>43835</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="7">
         <v>43895</v>
       </c>
-      <c r="O17" s="8">
+      <c r="O17" s="7">
         <v>1000000</v>
       </c>
-      <c r="P17" s="8" t="str">
+      <c r="P17" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="Q17" s="8">
+      <c r="Q17" s="7">
         <v>-1380000</v>
       </c>
-      <c r="R17" s="8" t="str">
+      <c r="R17" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="S17" s="8">
+      <c r="S17" s="7">
         <v>1.38</v>
       </c>
-      <c r="T17" s="8" t="b">
+      <c r="T17" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="U17" s="8">
+      <c r="U17" s="7">
         <v>43835</v>
       </c>
-      <c r="V17" s="8">
+      <c r="V17" s="7">
         <v>0</v>
       </c>
-      <c r="W17" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="X17" s="8" t="str">
-        <v>LUID_00004E5I,id-fx-swap-1</v>
-      </c>
-      <c r="Y17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="8" t="str">
+      <c r="W17" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="X17" s="7" t="str">
+        <v>id-fx-swap-1,LUID_00004E5I</v>
+      </c>
+      <c r="Y17" s="7" t="str">
         <v>ProperlyDefinedFXSwap1</v>
+      </c>
+      <c r="Z17" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA17" s="1" t="str">
+        <v/>
       </c>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
@@ -3498,80 +3479,80 @@
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>43790</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>43970</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>100000000</v>
       </c>
-      <c r="F18" s="8" t="str">
+      <c r="F18" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>-128863000</v>
       </c>
-      <c r="H18" s="8" t="str">
+      <c r="H18" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <v>1.2886299999999999</v>
       </c>
-      <c r="J18" s="8" t="b">
+      <c r="J18" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="7">
         <v>43790</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="7">
         <v>0</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18" s="7">
         <v>43790</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="7">
         <v>43972</v>
       </c>
-      <c r="O18" s="8">
+      <c r="O18" s="7">
         <v>50000000</v>
       </c>
-      <c r="P18" s="8" t="str">
+      <c r="P18" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="Q18" s="8">
+      <c r="Q18" s="7">
         <v>-64431500</v>
       </c>
-      <c r="R18" s="8" t="str">
+      <c r="R18" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="S18" s="8">
+      <c r="S18" s="7">
         <v>1.2886299999999999</v>
       </c>
-      <c r="T18" s="8" t="b">
+      <c r="T18" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="U18" s="8">
+      <c r="U18" s="7">
         <v>43790</v>
       </c>
-      <c r="V18" s="8">
+      <c r="V18" s="7">
         <v>0</v>
       </c>
-      <c r="W18" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="X18" s="8" t="str">
-        <v>LUID_00017MQ2,MyExcelSwap</v>
-      </c>
-      <c r="Y18" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="8" t="str">
-        <v>ExcelSwap</v>
+      <c r="W18" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="X18" s="7" t="str">
+        <v>MyExcelSwap,LUID_00017MQ2</v>
+      </c>
+      <c r="Y18" s="7" t="str">
+        <v>ExcelSwapUpdate</v>
+      </c>
+      <c r="Z18" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA18" s="1" t="str">
+        <v/>
       </c>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
@@ -3579,79 +3560,79 @@
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA19" s="8" t="str">
+      <c r="C19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z19" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA19" s="1" t="str">
         <v/>
       </c>
       <c r="AB19" s="1"/>
@@ -3660,79 +3641,79 @@
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA20" s="8" t="str">
+      <c r="C20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA20" s="1" t="str">
         <v/>
       </c>
       <c r="AB20" s="1"/>
@@ -3741,79 +3722,79 @@
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA21" s="8" t="str">
+      <c r="C21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z21" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA21" s="1" t="str">
         <v/>
       </c>
       <c r="AB21" s="1"/>
@@ -3822,79 +3803,79 @@
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA22" s="8" t="str">
+      <c r="C22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA22" s="1" t="str">
         <v/>
       </c>
       <c r="AB22" s="1"/>
@@ -3903,79 +3884,79 @@
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA23" s="8" t="str">
+      <c r="C23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA23" s="1" t="str">
         <v/>
       </c>
       <c r="AB23" s="1"/>
@@ -3984,79 +3965,79 @@
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA24" s="8" t="str">
+      <c r="C24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z24" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA24" s="1" t="str">
         <v/>
       </c>
       <c r="AB24" s="1"/>
@@ -4065,79 +4046,79 @@
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA25" s="8" t="str">
+      <c r="C25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z25" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA25" s="1" t="str">
         <v/>
       </c>
       <c r="AB25" s="1"/>
@@ -4146,79 +4127,79 @@
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA26" s="8" t="str">
+      <c r="C26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z26" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA26" s="1" t="str">
         <v/>
       </c>
       <c r="AB26" s="1"/>
@@ -4227,79 +4208,79 @@
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA27" s="8" t="str">
+      <c r="C27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z27" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA27" s="1" t="str">
         <v/>
       </c>
       <c r="AB27" s="1"/>
@@ -4370,7 +4351,7 @@
     <row r="30" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -4444,10 +4425,10 @@
         <v>9</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>22</v>
@@ -4503,291 +4484,287 @@
       <c r="Y32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Z32" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA32" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="8"/>
-      <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-      <c r="AA34" s="8"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-      <c r="AA37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="8"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="8"/>
-      <c r="AA38" s="8"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-      <c r="AA39" s="8"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-      <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-      <c r="AA40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="8"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-      <c r="AA41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
     </row>
@@ -4859,31 +4836,31 @@
     </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name" sqref="C32" xr:uid="{90964898-6A50-42A4-A407-2C38FCE3163A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Types" sqref="D32" xr:uid="{8AD2BD29-C252-461C-81B8-23C4D02A5783}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Ids" sqref="E32" xr:uid="{74F30A5B-D083-4651-882E-0D8B895BFB72}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LookThroughPortfolioId Scope" sqref="F32" xr:uid="{83AAE353-95AE-4290-B8A6-319A7BC31571}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LookThroughPortfolioId Code" sqref="G32" xr:uid="{14125927-AE07-4F79-996F-E9F6A78A8C65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearStartDate" sqref="H32" xr:uid="{9853CD87-24C8-4AC9-B27B-381D24CFFBE2}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearMaturityDate" sqref="I32" xr:uid="{35CFF59C-ED80-4384-A2D4-43E09AD39A53}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearDomAmount" sqref="J32" xr:uid="{C1181864-CC7E-4F38-B98E-61F906CC2D87}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearDomCcy" sqref="K32" xr:uid="{150AD7C1-F6AA-4784-83E1-8D7F6253EFFF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFgnAmount" sqref="L32" xr:uid="{1C702FD4-DB49-4B51-8F04-F5C31A66EF65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFgnCcy" sqref="M32" xr:uid="{728AC5BF-C083-45B1-8ABC-DF3FB67C1D65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearRefSpotRate" sqref="N32" xr:uid="{41D0F7CA-CB1A-452C-8CAC-58DB797F2B79}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearIsNdf" sqref="O32" xr:uid="{52F9125E-7702-434A-AC65-9E60FACE62DA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFixingDate" sqref="P32" xr:uid="{19CF1615-0B9F-4FA3-BB5C-49F569ABF2AB}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearSettlementCcy" sqref="Q32" xr:uid="{725661D4-958D-49D6-902A-C4DDBA6A3163}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarStartDate" sqref="R32" xr:uid="{CEE78929-9A41-44EB-9F43-5AD06462B324}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarMaturityDate" sqref="S32" xr:uid="{F42348B6-3041-4AE2-9E68-07F0237A083E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarDomAmount" sqref="T32" xr:uid="{8883C7AF-3463-4C9B-9330-9AE7EDCBBD56}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarDomCcy" sqref="U32" xr:uid="{2DC41E1E-4302-4BE1-9CDA-4BFFD4785D56}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFgnAmount" sqref="V32" xr:uid="{E4D796FC-0F15-49D8-B27A-0D2E81D45132}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFgnCcy" sqref="W32" xr:uid="{E9BD797A-7F53-4C61-9828-766BEDFAD568}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarRefSpotRate" sqref="X32" xr:uid="{CF405A83-357D-4F4F-92B5-334D82BC67B4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarIsNdf" sqref="Y32" xr:uid="{039641DE-88AB-4A09-A04E-26869758AE4F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFixingDate" sqref="Z32" xr:uid="{51D3CF76-0FF8-415C-AA02-08414034D391}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarSettlementCcy" sqref="AA32" xr:uid="{BC24EC2D-82E8-49E3-B152-56AC8D6353AF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name" sqref="C32" xr:uid="{C0606741-901B-4788-A8C4-DF4BA9A21AD5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Types" sqref="D32" xr:uid="{8E69A5A4-CC06-4CAC-9639-B3E2E010134F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Ids" sqref="E32" xr:uid="{E3AF64E3-8B39-4BCC-A8E7-E49F5E092CB6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearStartDate" sqref="F32" xr:uid="{DAC9DFEB-7577-48B9-8EFF-E21B89A2AF6C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearMaturityDate" sqref="G32" xr:uid="{9919D987-07C2-4504-B1D2-BED99EA34AEE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearDomAmount" sqref="H32" xr:uid="{C0FDD185-D37C-49E0-9A64-EA6C3468D97B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearDomCcy" sqref="I32" xr:uid="{411BD543-E23F-41B4-96EE-342DE512C11E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFgnAmount" sqref="J32" xr:uid="{A926503F-88F1-43B7-82E9-E8D1D8E5A73D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFgnCcy" sqref="K32" xr:uid="{3FDDB716-6D74-4721-9F43-11717312EA25}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearRefSpotRate" sqref="L32" xr:uid="{AF749B97-71F8-43E8-A544-4F82DE8BC690}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearIsNdf" sqref="M32" xr:uid="{6669FAD6-D630-45AB-8DEF-6D06173B361E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFixingDate" sqref="N32" xr:uid="{FD81C621-CDFF-4A76-B24B-1FBD986FE6BA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearSettlementCcy" sqref="O32" xr:uid="{DDF52DC9-0DF6-46EC-9DD4-728BCA7031DD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarStartDate" sqref="P32" xr:uid="{94E081C3-A528-470F-9A3B-A2450C5EC3E2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarMaturityDate" sqref="Q32" xr:uid="{EA7F0344-4D49-43BA-A278-A14F79732AD5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarDomAmount" sqref="R32" xr:uid="{AE0FC776-F139-4CB3-8F0F-EA34876D53C3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarDomCcy" sqref="S32" xr:uid="{9022B845-CFC4-4D5B-89B4-D0FFECDA5B54}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFgnAmount" sqref="T32" xr:uid="{951D9CEF-8D51-45F1-B118-96404C02E269}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFgnCcy" sqref="U32" xr:uid="{6764D403-3C60-4F6E-BC5E-40BF55CF530D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarRefSpotRate" sqref="V32" xr:uid="{8CE66E50-5FAF-4DF9-B1BA-FED7D6FF4BFC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarIsNdf" sqref="W32" xr:uid="{0E36B9A2-C13F-4BA9-9F8B-8A356CAC9C49}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFixingDate" sqref="X32" xr:uid="{43395E3B-F6E9-446A-845A-E9F506070B52}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarSettlementCcy" sqref="Y32" xr:uid="{06A92193-7ED0-425E-A154-3AB964954CEA}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CTECH-887 Update sheets to reflect column changes (#27)
</commit_message>
<xml_diff>
--- a/LUSID Excel - Manage instruments with economic definitions.xlsx
+++ b/LUSID Excel - Manage instruments with economic definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2CBBF2-F06C-4DC1-955B-35B6F4DFD530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DD4811-088C-4500-8B5F-34E374E521ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{610DF3B5-2DE7-41D6-946E-DDB270968A5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{610DF3B5-2DE7-41D6-946E-DDB270968A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="FxForwards" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>This sheet allows you to:</t>
   </si>
@@ -88,12 +88,6 @@
   </si>
   <si>
     <t>Instrument Ids</t>
-  </si>
-  <si>
-    <t>LookThroughPortfolioId Scope</t>
-  </si>
-  <si>
-    <t>LookThroughPortfolioId Code</t>
   </si>
   <si>
     <t>StartDate</t>
@@ -199,9 +193,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -316,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -328,13 +319,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -358,498 +343,498 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.18df948ffd4747e49d738fb50ed12bec">
+    <main first="rtdsrv.9ab47963834640bc914c733d5ccad4d8">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>af43bf5d-e2f3-4973-9fa8-962672089b30</stp>
+        <stp>f4456094-26c6-4647-beed-513e0c6fc7a2</stp>
+        <tr r="L23" s="2"/>
+        <tr r="R27" s="2"/>
+        <tr r="S19" s="2"/>
+        <tr r="K21" s="2"/>
+        <tr r="O16" s="2"/>
+        <tr r="V23" s="2"/>
+        <tr r="I17" s="2"/>
+        <tr r="L16" s="2"/>
+        <tr r="V24" s="2"/>
+        <tr r="E18" s="2"/>
+        <tr r="W19" s="2"/>
+        <tr r="O21" s="2"/>
+        <tr r="O27" s="2"/>
+        <tr r="Z24" s="2"/>
+        <tr r="D26" s="2"/>
+        <tr r="X23" s="2"/>
+        <tr r="D27" s="2"/>
+        <tr r="S24" s="2"/>
+        <tr r="X17" s="2"/>
+        <tr r="Y24" s="2"/>
+        <tr r="R24" s="2"/>
+        <tr r="P24" s="2"/>
+        <tr r="AA20" s="2"/>
+        <tr r="S25" s="2"/>
+        <tr r="U19" s="2"/>
+        <tr r="M21" s="2"/>
+        <tr r="J25" s="2"/>
+        <tr r="J20" s="2"/>
+        <tr r="C23" s="2"/>
+        <tr r="K19" s="2"/>
+        <tr r="I19" s="2"/>
+        <tr r="F19" s="2"/>
+        <tr r="W24" s="2"/>
+        <tr r="C22" s="2"/>
+        <tr r="V17" s="2"/>
+        <tr r="AA18" s="2"/>
+        <tr r="Z27" s="2"/>
+        <tr r="Y22" s="2"/>
+        <tr r="P22" s="2"/>
+        <tr r="G26" s="2"/>
+        <tr r="Y26" s="2"/>
+        <tr r="P25" s="2"/>
+        <tr r="M25" s="2"/>
+        <tr r="T23" s="2"/>
+        <tr r="P20" s="2"/>
+        <tr r="S27" s="2"/>
+        <tr r="T27" s="2"/>
+        <tr r="T17" s="2"/>
+        <tr r="AA22" s="2"/>
+        <tr r="K22" s="2"/>
+        <tr r="V21" s="2"/>
+        <tr r="L17" s="2"/>
+        <tr r="AA21" s="2"/>
+        <tr r="C19" s="2"/>
+        <tr r="Q22" s="2"/>
+        <tr r="V22" s="2"/>
+        <tr r="D19" s="2"/>
+        <tr r="Z25" s="2"/>
+        <tr r="M18" s="2"/>
+        <tr r="O20" s="2"/>
+        <tr r="Y20" s="2"/>
+        <tr r="D17" s="2"/>
+        <tr r="R26" s="2"/>
+        <tr r="V26" s="2"/>
+        <tr r="S21" s="2"/>
+        <tr r="W20" s="2"/>
+        <tr r="J27" s="2"/>
+        <tr r="M24" s="2"/>
+        <tr r="Z20" s="2"/>
+        <tr r="S16" s="2"/>
+        <tr r="C27" s="2"/>
+        <tr r="P16" s="2"/>
+        <tr r="E23" s="2"/>
+        <tr r="H25" s="2"/>
+        <tr r="W23" s="2"/>
+        <tr r="J18" s="2"/>
+        <tr r="W16" s="2"/>
+        <tr r="U21" s="2"/>
+        <tr r="I18" s="2"/>
+        <tr r="F20" s="2"/>
+        <tr r="N26" s="2"/>
+        <tr r="K18" s="2"/>
+        <tr r="H21" s="2"/>
+        <tr r="U20" s="2"/>
+        <tr r="Q17" s="2"/>
+        <tr r="J26" s="2"/>
+        <tr r="N17" s="2"/>
+        <tr r="Y17" s="2"/>
+        <tr r="E19" s="2"/>
+        <tr r="F22" s="2"/>
+        <tr r="E17" s="2"/>
+        <tr r="H16" s="2"/>
+        <tr r="P26" s="2"/>
+        <tr r="L19" s="2"/>
+        <tr r="M23" s="2"/>
+        <tr r="U18" s="2"/>
+        <tr r="P27" s="2"/>
+        <tr r="L27" s="2"/>
+        <tr r="AA24" s="2"/>
+        <tr r="D24" s="2"/>
+        <tr r="D22" s="2"/>
+        <tr r="P21" s="2"/>
+        <tr r="H22" s="2"/>
+        <tr r="G25" s="2"/>
+        <tr r="I25" s="2"/>
+        <tr r="O19" s="2"/>
+        <tr r="J22" s="2"/>
+        <tr r="AA27" s="2"/>
+        <tr r="V20" s="2"/>
+        <tr r="C24" s="2"/>
+        <tr r="Q25" s="2"/>
+        <tr r="Z23" s="2"/>
+        <tr r="U22" s="2"/>
+        <tr r="C16" s="2"/>
+        <tr r="Q21" s="2"/>
+        <tr r="W22" s="2"/>
+        <tr r="H17" s="2"/>
+        <tr r="D18" s="2"/>
+        <tr r="M17" s="2"/>
+        <tr r="H18" s="2"/>
+        <tr r="N23" s="2"/>
+        <tr r="G22" s="2"/>
+        <tr r="T24" s="2"/>
+        <tr r="M16" s="2"/>
+        <tr r="L26" s="2"/>
+        <tr r="AA17" s="2"/>
+        <tr r="L21" s="2"/>
+        <tr r="D21" s="2"/>
+        <tr r="D25" s="2"/>
+        <tr r="C20" s="2"/>
+        <tr r="T26" s="2"/>
+        <tr r="AA25" s="2"/>
+        <tr r="X18" s="2"/>
+        <tr r="W27" s="2"/>
+        <tr r="G18" s="2"/>
+        <tr r="X25" s="2"/>
+        <tr r="X22" s="2"/>
+        <tr r="F17" s="2"/>
+        <tr r="M19" s="2"/>
+        <tr r="S22" s="2"/>
+        <tr r="W26" s="2"/>
+        <tr r="I27" s="2"/>
+        <tr r="O26" s="2"/>
+        <tr r="Z19" s="2"/>
+        <tr r="J19" s="2"/>
+        <tr r="X20" s="2"/>
+        <tr r="Y25" s="2"/>
+        <tr r="G20" s="2"/>
+        <tr r="S20" s="2"/>
+        <tr r="E27" s="2"/>
+        <tr r="J21" s="2"/>
+        <tr r="H19" s="2"/>
+        <tr r="K25" s="2"/>
+        <tr r="Z21" s="2"/>
+        <tr r="Z26" s="2"/>
+        <tr r="T19" s="2"/>
+        <tr r="X21" s="2"/>
+        <tr r="K23" s="2"/>
+        <tr r="E22" s="2"/>
+        <tr r="W18" s="2"/>
+        <tr r="X27" s="2"/>
+        <tr r="H23" s="2"/>
+        <tr r="P19" s="2"/>
+        <tr r="AA19" s="2"/>
+        <tr r="J17" s="2"/>
+        <tr r="U17" s="2"/>
+        <tr r="Q19" s="2"/>
+        <tr r="E16" s="2"/>
+        <tr r="G16" s="2"/>
+        <tr r="I16" s="2"/>
+        <tr r="W21" s="2"/>
+        <tr r="G21" s="2"/>
+        <tr r="Q24" s="2"/>
+        <tr r="F18" s="2"/>
+        <tr r="Z16" s="2"/>
+        <tr r="V25" s="2"/>
+        <tr r="X16" s="2"/>
+        <tr r="G24" s="2"/>
+        <tr r="N20" s="2"/>
+        <tr r="W25" s="2"/>
+        <tr r="R21" s="2"/>
+        <tr r="T16" s="2"/>
+        <tr r="O23" s="2"/>
+        <tr r="F27" s="2"/>
+        <tr r="U24" s="2"/>
+        <tr r="H24" s="2"/>
+        <tr r="C17" s="2"/>
+        <tr r="R22" s="2"/>
+        <tr r="N24" s="2"/>
+        <tr r="L25" s="2"/>
+        <tr r="H27" s="2"/>
+        <tr r="T22" s="2"/>
+        <tr r="D20" s="2"/>
+        <tr r="M20" s="2"/>
+        <tr r="P18" s="2"/>
+        <tr r="N21" s="2"/>
+        <tr r="D23" s="2"/>
+        <tr r="M22" s="2"/>
+        <tr r="C26" s="2"/>
+        <tr r="F16" s="2"/>
+        <tr r="S17" s="2"/>
+        <tr r="P23" s="2"/>
+        <tr r="AA26" s="2"/>
+        <tr r="N27" s="2"/>
+        <tr r="H20" s="2"/>
+        <tr r="D16" s="2"/>
+        <tr r="Z22" s="2"/>
+        <tr r="Z17" s="2"/>
+        <tr r="Y27" s="2"/>
+        <tr r="O18" s="2"/>
+        <tr r="K16" s="2"/>
+        <tr r="K20" s="2"/>
+        <tr r="I23" s="2"/>
+        <tr r="R20" s="2"/>
         <tr r="X24" s="2"/>
         <tr r="H26" s="2"/>
-        <tr r="U17" s="2"/>
-        <tr r="H17" s="2"/>
-        <tr r="O26" s="2"/>
-        <tr r="I16" s="2"/>
-        <tr r="N21" s="2"/>
+        <tr r="L18" s="2"/>
+        <tr r="G27" s="2"/>
+        <tr r="G17" s="2"/>
+        <tr r="K24" s="2"/>
+        <tr r="AA23" s="2"/>
+        <tr r="O22" s="2"/>
+        <tr r="F25" s="2"/>
+        <tr r="AA16" s="2"/>
+        <tr r="R23" s="2"/>
+        <tr r="S23" s="2"/>
+        <tr r="C18" s="2"/>
+        <tr r="N25" s="2"/>
+        <tr r="M27" s="2"/>
+        <tr r="G19" s="2"/>
+        <tr r="Q26" s="2"/>
+        <tr r="I21" s="2"/>
+        <tr r="T18" s="2"/>
+        <tr r="I24" s="2"/>
+        <tr r="Q23" s="2"/>
+        <tr r="V18" s="2"/>
+        <tr r="Y19" s="2"/>
+        <tr r="I20" s="2"/>
+        <tr r="C21" s="2"/>
+        <tr r="R18" s="2"/>
+        <tr r="Q16" s="2"/>
+        <tr r="N16" s="2"/>
+        <tr r="Q27" s="2"/>
+        <tr r="F24" s="2"/>
+        <tr r="N18" s="2"/>
+        <tr r="S26" s="2"/>
+        <tr r="O25" s="2"/>
+        <tr r="Z18" s="2"/>
+        <tr r="I22" s="2"/>
+        <tr r="F23" s="2"/>
+        <tr r="L24" s="2"/>
+        <tr r="K27" s="2"/>
         <tr r="T20" s="2"/>
-        <tr r="T18" s="2"/>
+        <tr r="U16" s="2"/>
+        <tr r="N19" s="2"/>
         <tr r="Q20" s="2"/>
+        <tr r="U23" s="2"/>
+        <tr r="P17" s="2"/>
+        <tr r="V16" s="2"/>
+        <tr r="F21" s="2"/>
+        <tr r="U27" s="2"/>
+        <tr r="U26" s="2"/>
+        <tr r="X19" s="2"/>
+        <tr r="R19" s="2"/>
+        <tr r="L20" s="2"/>
+        <tr r="K17" s="2"/>
+        <tr r="T21" s="2"/>
+        <tr r="V27" s="2"/>
+        <tr r="Y18" s="2"/>
+        <tr r="E24" s="2"/>
+        <tr r="Y23" s="2"/>
+        <tr r="M26" s="2"/>
+        <tr r="C25" s="2"/>
+        <tr r="R25" s="2"/>
+        <tr r="J16" s="2"/>
+        <tr r="K26" s="2"/>
+        <tr r="J24" s="2"/>
+        <tr r="J23" s="2"/>
+        <tr r="T25" s="2"/>
+        <tr r="G23" s="2"/>
         <tr r="N22" s="2"/>
-        <tr r="T23" s="2"/>
-        <tr r="Z24" s="2"/>
-        <tr r="M21" s="2"/>
-        <tr r="Q22" s="2"/>
-        <tr r="E23" s="2"/>
-        <tr r="O19" s="2"/>
-        <tr r="P19" s="2"/>
-        <tr r="D20" s="2"/>
-        <tr r="D18" s="2"/>
-        <tr r="Z19" s="2"/>
-        <tr r="W21" s="2"/>
-        <tr r="D23" s="2"/>
-        <tr r="J24" s="2"/>
-        <tr r="I24" s="2"/>
-        <tr r="U23" s="2"/>
         <tr r="Y16" s="2"/>
-        <tr r="L16" s="2"/>
-        <tr r="K22" s="2"/>
-        <tr r="J25" s="2"/>
-        <tr r="V22" s="2"/>
-        <tr r="H25" s="2"/>
-        <tr r="E17" s="2"/>
-        <tr r="AA16" s="2"/>
-        <tr r="M19" s="2"/>
-        <tr r="M17" s="2"/>
-        <tr r="J19" s="2"/>
-        <tr r="G21" s="2"/>
-        <tr r="M22" s="2"/>
-        <tr r="S23" s="2"/>
-        <tr r="Q23" s="2"/>
-        <tr r="P17" s="2"/>
         <tr r="V19" s="2"/>
-        <tr r="L23" s="2"/>
-        <tr r="D26" s="2"/>
-        <tr r="J20" s="2"/>
-        <tr r="D19" s="2"/>
-        <tr r="W23" s="2"/>
-        <tr r="F25" s="2"/>
-        <tr r="L25" s="2"/>
-        <tr r="C24" s="2"/>
-        <tr r="H18" s="2"/>
-        <tr r="X20" s="2"/>
-        <tr r="Q24" s="2"/>
-        <tr r="C26" s="2"/>
-        <tr r="G27" s="2"/>
-        <tr r="V18" s="2"/>
-        <tr r="V16" s="2"/>
         <tr r="S18" s="2"/>
-        <tr r="P20" s="2"/>
-        <tr r="V21" s="2"/>
-        <tr r="C23" s="2"/>
-        <tr r="Z25" s="2"/>
-        <tr r="J18" s="2"/>
-        <tr r="X25" s="2"/>
-        <tr r="J22" s="2"/>
-        <tr r="Q19" s="2"/>
-        <tr r="N23" s="2"/>
-        <tr r="Y25" s="2"/>
-        <tr r="F18" s="2"/>
-        <tr r="F16" s="2"/>
-        <tr r="C18" s="2"/>
-        <tr r="Y19" s="2"/>
-        <tr r="F21" s="2"/>
         <tr r="L22" s="2"/>
-        <tr r="V24" s="2"/>
-        <tr r="X23" s="2"/>
-        <tr r="K19" s="2"/>
-        <tr r="M18" s="2"/>
-        <tr r="W16" s="2"/>
-        <tr r="H23" s="2"/>
-        <tr r="X22" s="2"/>
-        <tr r="M20" s="2"/>
-        <tr r="G22" s="2"/>
-        <tr r="G20" s="2"/>
-        <tr r="Z16" s="2"/>
-        <tr r="S17" s="2"/>
-        <tr r="J23" s="2"/>
-        <tr r="I20" s="2"/>
-        <tr r="U27" s="2"/>
         <tr r="O17" s="2"/>
-        <tr r="R27" s="2"/>
-        <tr r="L17" s="2"/>
-        <tr r="I19" s="2"/>
-        <tr r="O20" s="2"/>
-        <tr r="U21" s="2"/>
-        <tr r="H22" s="2"/>
-        <tr r="AA19" s="2"/>
-        <tr r="Q25" s="2"/>
-        <tr r="T24" s="2"/>
-        <tr r="S20" s="2"/>
-        <tr r="V25" s="2"/>
-        <tr r="P23" s="2"/>
-        <tr r="G17" s="2"/>
-        <tr r="C21" s="2"/>
-        <tr r="U26" s="2"/>
         <tr r="W17" s="2"/>
-        <tr r="S27" s="2"/>
-        <tr r="D27" s="2"/>
-        <tr r="F19" s="2"/>
-        <tr r="Y20" s="2"/>
-        <tr r="I18" s="2"/>
-        <tr r="J16" s="2"/>
-        <tr r="H27" s="2"/>
-        <tr r="S22" s="2"/>
-        <tr r="M16" s="2"/>
-        <tr r="E27" s="2"/>
-        <tr r="X16" s="2"/>
-        <tr r="AA26" s="2"/>
-        <tr r="U16" s="2"/>
-        <tr r="R18" s="2"/>
-        <tr r="X19" s="2"/>
         <tr r="E21" s="2"/>
-        <tr r="E18" s="2"/>
-        <tr r="AA21" s="2"/>
-        <tr r="W24" s="2"/>
-        <tr r="D17" s="2"/>
-        <tr r="F20" s="2"/>
-        <tr r="N24" s="2"/>
-        <tr r="AA27" s="2"/>
-        <tr r="Z23" s="2"/>
-        <tr r="L26" s="2"/>
-        <tr r="J21" s="2"/>
-        <tr r="G24" s="2"/>
-        <tr r="N27" s="2"/>
-        <tr r="N25" s="2"/>
-        <tr r="Q16" s="2"/>
-        <tr r="R19" s="2"/>
         <tr r="R17" s="2"/>
-        <tr r="S19" s="2"/>
-        <tr r="S24" s="2"/>
-        <tr r="C22" s="2"/>
-        <tr r="R26" s="2"/>
-        <tr r="N26" s="2"/>
-        <tr r="H16" s="2"/>
-        <tr r="K26" s="2"/>
-        <tr r="E16" s="2"/>
-        <tr r="AA17" s="2"/>
-        <tr r="H19" s="2"/>
-        <tr r="N20" s="2"/>
-        <tr r="H20" s="2"/>
-        <tr r="K24" s="2"/>
-        <tr r="N16" s="2"/>
-        <tr r="L20" s="2"/>
         <tr r="E26" s="2"/>
-        <tr r="T27" s="2"/>
-        <tr r="X17" s="2"/>
-        <tr r="V17" s="2"/>
-        <tr r="V26" s="2"/>
-        <tr r="K18" s="2"/>
-        <tr r="P26" s="2"/>
-        <tr r="L18" s="2"/>
-        <tr r="U22" s="2"/>
-        <tr r="L21" s="2"/>
-        <tr r="K25" s="2"/>
-        <tr r="W25" s="2"/>
-        <tr r="D16" s="2"/>
-        <tr r="T25" s="2"/>
-        <tr r="Q27" s="2"/>
-        <tr r="K17" s="2"/>
         <tr r="Q18" s="2"/>
-        <tr r="W19" s="2"/>
-        <tr r="Y24" s="2"/>
-        <tr r="AA18" s="2"/>
-        <tr r="S21" s="2"/>
-        <tr r="H21" s="2"/>
-        <tr r="L19" s="2"/>
-        <tr r="K27" s="2"/>
-        <tr r="W26" s="2"/>
-        <tr r="D21" s="2"/>
-        <tr r="Z21" s="2"/>
-        <tr r="R21" s="2"/>
-        <tr r="Z22" s="2"/>
-        <tr r="M27" s="2"/>
-        <tr r="F24" s="2"/>
-        <tr r="T21" s="2"/>
         <tr r="E25" s="2"/>
-        <tr r="T17" s="2"/>
-        <tr r="R24" s="2"/>
-        <tr r="Z27" s="2"/>
-        <tr r="W20" s="2"/>
-        <tr r="U20" s="2"/>
-        <tr r="M23" s="2"/>
-        <tr r="G25" s="2"/>
-        <tr r="C16" s="2"/>
-        <tr r="D25" s="2"/>
-        <tr r="Z26" s="2"/>
-        <tr r="T16" s="2"/>
-        <tr r="Z17" s="2"/>
-        <tr r="G19" s="2"/>
-        <tr r="N18" s="2"/>
-        <tr r="V27" s="2"/>
         <tr r="O24" s="2"/>
-        <tr r="K21" s="2"/>
-        <tr r="C19" s="2"/>
-        <tr r="Y22" s="2"/>
-        <tr r="J27" s="2"/>
-        <tr r="Q17" s="2"/>
-        <tr r="U18" s="2"/>
-        <tr r="R23" s="2"/>
-        <tr r="G16" s="2"/>
-        <tr r="C20" s="2"/>
-        <tr r="T19" s="2"/>
-        <tr r="O23" s="2"/>
-        <tr r="Y27" s="2"/>
-        <tr r="AA23" s="2"/>
-        <tr r="S26" s="2"/>
-        <tr r="Y18" s="2"/>
         <tr r="E20" s="2"/>
-        <tr r="O21" s="2"/>
-        <tr r="P24" s="2"/>
-        <tr r="P22" s="2"/>
-        <tr r="M24" s="2"/>
-        <tr r="J26" s="2"/>
-        <tr r="P27" s="2"/>
-        <tr r="J17" s="2"/>
-        <tr r="P18" s="2"/>
-        <tr r="T26" s="2"/>
-        <tr r="X21" s="2"/>
-        <tr r="F27" s="2"/>
-        <tr r="O18" s="2"/>
-        <tr r="Q26" s="2"/>
-        <tr r="O25" s="2"/>
-        <tr r="E24" s="2"/>
         <tr r="U25" s="2"/>
-        <tr r="O16" s="2"/>
-        <tr r="AA20" s="2"/>
-        <tr r="G26" s="2"/>
-        <tr r="Z20" s="2"/>
-        <tr r="N17" s="2"/>
-        <tr r="L27" s="2"/>
-        <tr r="F17" s="2"/>
-        <tr r="Q21" s="2"/>
-        <tr r="AA25" s="2"/>
-        <tr r="K23" s="2"/>
-        <tr r="U24" s="2"/>
-        <tr r="K16" s="2"/>
-        <tr r="N19" s="2"/>
-        <tr r="Z18" s="2"/>
-        <tr r="Y23" s="2"/>
         <tr r="Y21" s="2"/>
-        <tr r="V23" s="2"/>
-        <tr r="S25" s="2"/>
-        <tr r="Y26" s="2"/>
-        <tr r="S16" s="2"/>
-        <tr r="Y17" s="2"/>
-        <tr r="AA24" s="2"/>
-        <tr r="V20" s="2"/>
-        <tr r="I27" s="2"/>
-        <tr r="X18" s="2"/>
-        <tr r="E22" s="2"/>
-        <tr r="H24" s="2"/>
-        <tr r="K20" s="2"/>
-        <tr r="G23" s="2"/>
-        <tr r="I22" s="2"/>
-        <tr r="M26" s="2"/>
         <tr r="F26" s="2"/>
-        <tr r="AA22" s="2"/>
-        <tr r="U19" s="2"/>
-        <tr r="P25" s="2"/>
-        <tr r="C27" s="2"/>
-        <tr r="E19" s="2"/>
-        <tr r="D24" s="2"/>
-        <tr r="T22" s="2"/>
-        <tr r="W22" s="2"/>
-        <tr r="W27" s="2"/>
-        <tr r="W18" s="2"/>
-        <tr r="C17" s="2"/>
-        <tr r="I23" s="2"/>
-        <tr r="I21" s="2"/>
-        <tr r="F23" s="2"/>
-        <tr r="C25" s="2"/>
         <tr r="I26" s="2"/>
-        <tr r="O27" s="2"/>
-        <tr r="I17" s="2"/>
-        <tr r="M25" s="2"/>
-        <tr r="P16" s="2"/>
-        <tr r="F22" s="2"/>
-        <tr r="D22" s="2"/>
-        <tr r="P21" s="2"/>
-        <tr r="I25" s="2"/>
-        <tr r="G18" s="2"/>
-        <tr r="X27" s="2"/>
-        <tr r="R22" s="2"/>
-        <tr r="R20" s="2"/>
-        <tr r="O22" s="2"/>
-        <tr r="L24" s="2"/>
-        <tr r="R25" s="2"/>
         <tr r="X26" s="2"/>
         <tr r="R16" s="2"/>
       </tp>
     </main>
-    <main first="rtdsrv.18df948ffd4747e49d738fb50ed12bec">
+    <main first="rtdsrv.9ab47963834640bc914c733d5ccad4d8">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>a909e5ee-15c7-43e3-9ee8-aa5852c79f7b</stp>
+        <stp>ef729c81-1fef-416c-b027-efd040b8e69d</stp>
+        <tr r="J17" s="1"/>
+        <tr r="L17" s="1"/>
+        <tr r="F18" s="1"/>
+        <tr r="H22" s="1"/>
+        <tr r="D20" s="1"/>
+        <tr r="E22" s="1"/>
+        <tr r="H17" s="1"/>
+        <tr r="G25" s="1"/>
+        <tr r="I27" s="1"/>
+        <tr r="F27" s="1"/>
+        <tr r="G16" s="1"/>
+        <tr r="L23" s="1"/>
+        <tr r="Q26" s="1"/>
+        <tr r="E23" s="1"/>
+        <tr r="I24" s="1"/>
+        <tr r="J24" s="1"/>
+        <tr r="F19" s="1"/>
+        <tr r="L19" s="1"/>
+        <tr r="J19" s="1"/>
+        <tr r="G21" s="1"/>
+        <tr r="P18" s="1"/>
         <tr r="L22" s="1"/>
-        <tr r="F27" s="1"/>
+        <tr r="H26" s="1"/>
+        <tr r="K25" s="1"/>
+        <tr r="D25" s="1"/>
+        <tr r="F26" s="1"/>
         <tr r="M26" s="1"/>
+        <tr r="E20" s="1"/>
+        <tr r="J16" s="1"/>
+        <tr r="E19" s="1"/>
+        <tr r="L21" s="1"/>
+        <tr r="N17" s="1"/>
+        <tr r="G26" s="1"/>
+        <tr r="F21" s="1"/>
+        <tr r="E18" s="1"/>
+        <tr r="I18" s="1"/>
+        <tr r="O19" s="1"/>
+        <tr r="M19" s="1"/>
+        <tr r="L24" s="1"/>
+        <tr r="P19" s="1"/>
+        <tr r="I23" s="1"/>
+        <tr r="F25" s="1"/>
+        <tr r="L27" s="1"/>
+        <tr r="Q24" s="1"/>
+        <tr r="I19" s="1"/>
+        <tr r="F20" s="1"/>
+        <tr r="F24" s="1"/>
+        <tr r="H23" s="1"/>
+        <tr r="Q18" s="1"/>
+        <tr r="C16" s="1"/>
+        <tr r="C22" s="1"/>
         <tr r="C20" s="1"/>
+        <tr r="O23" s="1"/>
+        <tr r="D27" s="1"/>
+        <tr r="Q20" s="1"/>
+        <tr r="G20" s="1"/>
+        <tr r="E25" s="1"/>
+        <tr r="K20" s="1"/>
+        <tr r="D16" s="1"/>
+        <tr r="O26" s="1"/>
+        <tr r="O22" s="1"/>
+        <tr r="L16" s="1"/>
+        <tr r="E24" s="1"/>
+        <tr r="Q23" s="1"/>
+        <tr r="F22" s="1"/>
+        <tr r="P20" s="1"/>
+        <tr r="Q17" s="1"/>
+        <tr r="J18" s="1"/>
+        <tr r="H20" s="1"/>
+        <tr r="I20" s="1"/>
+        <tr r="D17" s="1"/>
+        <tr r="C24" s="1"/>
+        <tr r="O27" s="1"/>
+        <tr r="F23" s="1"/>
+        <tr r="C18" s="1"/>
+        <tr r="D19" s="1"/>
+        <tr r="M25" s="1"/>
+        <tr r="K27" s="1"/>
+        <tr r="E26" s="1"/>
+        <tr r="P16" s="1"/>
+        <tr r="K22" s="1"/>
+        <tr r="L20" s="1"/>
+        <tr r="K21" s="1"/>
+        <tr r="M20" s="1"/>
+        <tr r="O17" s="1"/>
+        <tr r="K18" s="1"/>
+        <tr r="P26" s="1"/>
+        <tr r="K23" s="1"/>
+        <tr r="N26" s="1"/>
+        <tr r="C26" s="1"/>
+        <tr r="J25" s="1"/>
+        <tr r="F17" s="1"/>
+        <tr r="H25" s="1"/>
+        <tr r="D24" s="1"/>
+        <tr r="D21" s="1"/>
+        <tr r="O20" s="1"/>
+        <tr r="O21" s="1"/>
+        <tr r="M21" s="1"/>
+        <tr r="M17" s="1"/>
+        <tr r="K19" s="1"/>
+        <tr r="P23" s="1"/>
+        <tr r="N19" s="1"/>
+        <tr r="E27" s="1"/>
+        <tr r="J22" s="1"/>
+        <tr r="L26" s="1"/>
+        <tr r="Q27" s="1"/>
+        <tr r="P24" s="1"/>
+        <tr r="C23" s="1"/>
+        <tr r="C19" s="1"/>
+        <tr r="G17" s="1"/>
+        <tr r="Q25" s="1"/>
+        <tr r="N18" s="1"/>
+        <tr r="O24" s="1"/>
+        <tr r="H18" s="1"/>
+        <tr r="H27" s="1"/>
+        <tr r="M24" s="1"/>
+        <tr r="D18" s="1"/>
+        <tr r="Q22" s="1"/>
+        <tr r="H16" s="1"/>
+        <tr r="M22" s="1"/>
+        <tr r="D23" s="1"/>
+        <tr r="C21" s="1"/>
+        <tr r="G22" s="1"/>
+        <tr r="H21" s="1"/>
+        <tr r="C25" s="1"/>
+        <tr r="L18" s="1"/>
+        <tr r="J26" s="1"/>
+        <tr r="I17" s="1"/>
+        <tr r="Q21" s="1"/>
+        <tr r="O25" s="1"/>
+        <tr r="I25" s="1"/>
+        <tr r="J21" s="1"/>
+        <tr r="M16" s="1"/>
+        <tr r="I16" s="1"/>
+        <tr r="P22" s="1"/>
+        <tr r="H24" s="1"/>
+        <tr r="G27" s="1"/>
+        <tr r="J20" s="1"/>
+        <tr r="D22" s="1"/>
+        <tr r="K17" s="1"/>
+        <tr r="G24" s="1"/>
+        <tr r="N25" s="1"/>
+        <tr r="K26" s="1"/>
+        <tr r="K16" s="1"/>
+        <tr r="K24" s="1"/>
+        <tr r="I21" s="1"/>
+        <tr r="Q19" s="1"/>
+        <tr r="N16" s="1"/>
+        <tr r="P25" s="1"/>
+        <tr r="I26" s="1"/>
+        <tr r="Q16" s="1"/>
+        <tr r="N23" s="1"/>
+        <tr r="D26" s="1"/>
+        <tr r="M27" s="1"/>
+        <tr r="N27" s="1"/>
+        <tr r="F16" s="1"/>
+        <tr r="O18" s="1"/>
+        <tr r="C17" s="1"/>
+        <tr r="E17" s="1"/>
+        <tr r="J27" s="1"/>
+        <tr r="P17" s="1"/>
         <tr r="M18" s="1"/>
-        <tr r="K20" s="1"/>
-        <tr r="J25" s="1"/>
-        <tr r="E24" s="1"/>
-        <tr r="Q25" s="1"/>
-        <tr r="O20" s="1"/>
-        <tr r="O24" s="1"/>
+        <tr r="L25" s="1"/>
         <tr r="P27" s="1"/>
-        <tr r="H24" s="1"/>
-        <tr r="D26" s="1"/>
+        <tr r="M23" s="1"/>
+        <tr r="N21" s="1"/>
+        <tr r="N22" s="1"/>
+        <tr r="H19" s="1"/>
+        <tr r="E21" s="1"/>
         <tr r="I22" s="1"/>
-        <tr r="P17" s="1"/>
-        <tr r="L17" s="1"/>
-        <tr r="G16" s="1"/>
-        <tr r="E20" s="1"/>
-        <tr r="P19" s="1"/>
-        <tr r="P24" s="1"/>
-        <tr r="D19" s="1"/>
-        <tr r="K27" s="1"/>
-        <tr r="Q23" s="1"/>
-        <tr r="K22" s="1"/>
-        <tr r="O21" s="1"/>
-        <tr r="H18" s="1"/>
-        <tr r="J26" s="1"/>
-        <tr r="G27" s="1"/>
-        <tr r="N22" s="1"/>
         <tr r="C27" s="1"/>
-        <tr r="O23" s="1"/>
-        <tr r="E22" s="1"/>
-        <tr r="L23" s="1"/>
-        <tr r="J16" s="1"/>
-        <tr r="I23" s="1"/>
-        <tr r="N16" s="1"/>
-        <tr r="L18" s="1"/>
-        <tr r="O26" s="1"/>
-        <tr r="F22" s="1"/>
-        <tr r="D24" s="1"/>
-        <tr r="M21" s="1"/>
-        <tr r="H27" s="1"/>
-        <tr r="Q16" s="1"/>
-        <tr r="J20" s="1"/>
-        <tr r="M27" s="1"/>
         <tr r="O16" s="1"/>
-        <tr r="K23" s="1"/>
-        <tr r="H26" s="1"/>
-        <tr r="Q26" s="1"/>
-        <tr r="E19" s="1"/>
-        <tr r="F25" s="1"/>
-        <tr r="D27" s="1"/>
-        <tr r="J21" s="1"/>
-        <tr r="C19" s="1"/>
-        <tr r="P20" s="1"/>
-        <tr r="L20" s="1"/>
-        <tr r="M17" s="1"/>
-        <tr r="M24" s="1"/>
-        <tr r="M16" s="1"/>
-        <tr r="D22" s="1"/>
-        <tr r="H19" s="1"/>
         <tr r="G18" s="1"/>
-        <tr r="L24" s="1"/>
-        <tr r="F18" s="1"/>
-        <tr r="E23" s="1"/>
-        <tr r="L21" s="1"/>
-        <tr r="L27" s="1"/>
-        <tr r="C22" s="1"/>
-        <tr r="C26" s="1"/>
-        <tr r="F17" s="1"/>
-        <tr r="Q17" s="1"/>
-        <tr r="N18" s="1"/>
-        <tr r="K19" s="1"/>
-        <tr r="D18" s="1"/>
-        <tr r="M23" s="1"/>
-        <tr r="K17" s="1"/>
-        <tr r="N27" s="1"/>
         <tr r="J23" s="1"/>
-        <tr r="Q19" s="1"/>
-        <tr r="H17" s="1"/>
-        <tr r="I24" s="1"/>
-        <tr r="N17" s="1"/>
-        <tr r="Q24" s="1"/>
-        <tr r="N26" s="1"/>
-        <tr r="I26" s="1"/>
-        <tr r="E26" s="1"/>
-        <tr r="J18" s="1"/>
-        <tr r="K21" s="1"/>
-        <tr r="P23" s="1"/>
-        <tr r="Q22" s="1"/>
-        <tr r="I17" s="1"/>
-        <tr r="G24" s="1"/>
-        <tr r="E21" s="1"/>
         <tr r="N24" s="1"/>
-        <tr r="F23" s="1"/>
-        <tr r="K25" s="1"/>
-        <tr r="J24" s="1"/>
-        <tr r="G26" s="1"/>
-        <tr r="I19" s="1"/>
-        <tr r="C18" s="1"/>
-        <tr r="C23" s="1"/>
-        <tr r="O22" s="1"/>
-        <tr r="H20" s="1"/>
-        <tr r="D21" s="1"/>
-        <tr r="N19" s="1"/>
-        <tr r="H16" s="1"/>
-        <tr r="I16" s="1"/>
-        <tr r="N25" s="1"/>
-        <tr r="F16" s="1"/>
         <tr r="G19" s="1"/>
-        <tr r="O25" s="1"/>
-        <tr r="G25" s="1"/>
-        <tr r="F19" s="1"/>
-        <tr r="F21" s="1"/>
-        <tr r="F20" s="1"/>
-        <tr r="I25" s="1"/>
-        <tr r="L25" s="1"/>
-        <tr r="H25" s="1"/>
-        <tr r="I20" s="1"/>
-        <tr r="M20" s="1"/>
-        <tr r="E27" s="1"/>
-        <tr r="M22" s="1"/>
-        <tr r="N23" s="1"/>
-        <tr r="K26" s="1"/>
-        <tr r="O18" s="1"/>
         <tr r="E16" s="1"/>
-        <tr r="D20" s="1"/>
-        <tr r="D25" s="1"/>
-        <tr r="L19" s="1"/>
-        <tr r="E18" s="1"/>
-        <tr r="F24" s="1"/>
-        <tr r="C25" s="1"/>
-        <tr r="D16" s="1"/>
-        <tr r="G17" s="1"/>
-        <tr r="D17" s="1"/>
-        <tr r="O17" s="1"/>
-        <tr r="J22" s="1"/>
-        <tr r="D23" s="1"/>
-        <tr r="N21" s="1"/>
-        <tr r="K16" s="1"/>
-        <tr r="C17" s="1"/>
         <tr r="G23" s="1"/>
-        <tr r="H21" s="1"/>
-        <tr r="I27" s="1"/>
-        <tr r="J19" s="1"/>
-        <tr r="I18" s="1"/>
-        <tr r="H23" s="1"/>
-        <tr r="E25" s="1"/>
-        <tr r="M25" s="1"/>
-        <tr r="P16" s="1"/>
-        <tr r="C24" s="1"/>
-        <tr r="K18" s="1"/>
-        <tr r="L26" s="1"/>
-        <tr r="C21" s="1"/>
-        <tr r="P22" s="1"/>
-        <tr r="K24" s="1"/>
-        <tr r="E17" s="1"/>
         <tr r="N20" s="1"/>
-        <tr r="G20" s="1"/>
-        <tr r="F26" s="1"/>
-        <tr r="G21" s="1"/>
-        <tr r="O19" s="1"/>
-        <tr r="Q18" s="1"/>
-        <tr r="P25" s="1"/>
-        <tr r="Q20" s="1"/>
-        <tr r="L16" s="1"/>
-        <tr r="O27" s="1"/>
-        <tr r="P26" s="1"/>
-        <tr r="Q27" s="1"/>
-        <tr r="G22" s="1"/>
-        <tr r="Q21" s="1"/>
-        <tr r="I21" s="1"/>
-        <tr r="J27" s="1"/>
         <tr r="P21" s="1"/>
-        <tr r="J17" s="1"/>
-        <tr r="H22" s="1"/>
-        <tr r="P18" s="1"/>
-        <tr r="M19" s="1"/>
-        <tr r="C16" s="1"/>
       </tp>
     </main>
   </volType>
@@ -1155,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F32773-32F6-4E82-8FD8-8EE0575AC374}">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1398,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5"/>
@@ -1471,7 +1456,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="5"/>
@@ -1529,7 +1514,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5"/>
@@ -1654,13 +1639,13 @@
         <v>Instrument Ids</v>
       </c>
       <c r="O16" s="6" t="str">
-        <v>LookThroughPortfolioId Scope</v>
-      </c>
-      <c r="P16" s="7" t="str">
-        <v>LookThroughPortfolioId Code</v>
-      </c>
-      <c r="Q16" s="6" t="str">
         <v>Name</v>
+      </c>
+      <c r="P16" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q16" s="1" t="str">
+        <v/>
       </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1675,50 +1660,50 @@
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>43790</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>43972</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>100000000</v>
       </c>
-      <c r="F17" s="8" t="str">
+      <c r="F17" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>-128863000</v>
       </c>
-      <c r="H17" s="8" t="str">
+      <c r="H17" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="7">
         <v>1.2886299999999999</v>
       </c>
-      <c r="J17" s="8" t="b">
+      <c r="J17" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="7">
         <v>43790</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="7">
         <v>0</v>
       </c>
-      <c r="M17" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N17" s="8" t="str">
-        <v>LUID_2W533GOV,FXFWD0001</v>
-      </c>
-      <c r="O17" s="8">
-        <v>0</v>
-      </c>
-      <c r="P17" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="8" t="str">
-        <v>FXFWD1-Update</v>
+      <c r="M17" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N17" s="7" t="str">
+        <v>FXFWD0001,LUID_2W533GOV</v>
+      </c>
+      <c r="O17" s="7" t="str">
+        <v>FXFWD1-UpdateTheSecond</v>
+      </c>
+      <c r="P17" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q17" s="1" t="str">
+        <v/>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -1733,50 +1718,50 @@
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>43790</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>43972</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>50000000</v>
       </c>
-      <c r="F18" s="8" t="str">
+      <c r="F18" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>-64431500</v>
       </c>
-      <c r="H18" s="8" t="str">
+      <c r="H18" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <v>1.2886299999999999</v>
       </c>
-      <c r="J18" s="8" t="b">
+      <c r="J18" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="7">
         <v>43790</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="7">
         <v>0</v>
       </c>
-      <c r="M18" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N18" s="8" t="str">
-        <v>LUID_1UDR6T2I,FXFWD0002</v>
-      </c>
-      <c r="O18" s="8">
-        <v>0</v>
-      </c>
-      <c r="P18" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="8" t="str">
+      <c r="M18" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N18" s="7" t="str">
+        <v>FXFWD0002,LUID_1UDR6T2I</v>
+      </c>
+      <c r="O18" s="7" t="str">
         <v>FXFWD2</v>
+      </c>
+      <c r="P18" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q18" s="1" t="str">
+        <v/>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1791,50 +1776,50 @@
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>43957.684771770837</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <v>44322.684771770837</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>1</v>
       </c>
-      <c r="F19" s="8" t="str">
+      <c r="F19" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>-1.3</v>
       </c>
-      <c r="H19" s="8" t="str">
+      <c r="H19" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="7">
         <v>1</v>
       </c>
-      <c r="J19" s="8" t="b">
+      <c r="J19" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="7">
         <v>43957.684771770837</v>
       </c>
-      <c r="L19" s="8">
+      <c r="L19" s="7">
         <v>0</v>
       </c>
-      <c r="M19" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N19" s="8" t="str">
-        <v>LUID_F0UY3CY8,FxForward-637243791205499396</v>
-      </c>
-      <c r="O19" s="8">
-        <v>0</v>
-      </c>
-      <c r="P19" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="8" t="str">
+      <c r="M19" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N19" s="7" t="str">
+        <v>FxForward-637243791205499396,LUID_F0UY3CY8</v>
+      </c>
+      <c r="O19" s="7" t="str">
         <v>FxForward-637243791205499396</v>
+      </c>
+      <c r="P19" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q19" s="1" t="str">
+        <v/>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -1849,50 +1834,50 @@
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>43983</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>43990</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>1</v>
       </c>
-      <c r="F20" s="8" t="str">
+      <c r="F20" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>-1.2508999999999999</v>
       </c>
-      <c r="H20" s="8" t="str">
+      <c r="H20" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="7">
         <v>1.2507999999999999</v>
       </c>
-      <c r="J20" s="8" t="b">
+      <c r="J20" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="7">
         <v>0</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="7">
         <v>0</v>
       </c>
-      <c r="M20" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N20" s="8" t="str">
-        <v>LUID_JW6AVI4S,gbp_usd_fwd_1w_12509</v>
-      </c>
-      <c r="O20" s="8">
-        <v>0</v>
-      </c>
-      <c r="P20" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="8" t="str">
+      <c r="M20" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N20" s="7" t="str">
+        <v>gbp_usd_fwd_1w_12509,LUID_JW6AVI4S</v>
+      </c>
+      <c r="O20" s="7" t="str">
         <v>GBP/USD 1W @ 1.2509</v>
+      </c>
+      <c r="P20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q20" s="1" t="str">
+        <v/>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -1907,50 +1892,50 @@
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>43868</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>44092</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>1</v>
       </c>
-      <c r="F21" s="8" t="str">
+      <c r="F21" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>-123</v>
       </c>
-      <c r="H21" s="8" t="str">
+      <c r="H21" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="7">
         <v>100</v>
       </c>
-      <c r="J21" s="8" t="b">
+      <c r="J21" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="7">
         <v>44061</v>
       </c>
-      <c r="L21" s="8">
+      <c r="L21" s="7">
         <v>0</v>
       </c>
-      <c r="M21" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N21" s="8" t="str">
-        <v>LUID_XHV68ZZA,FxForward_uniqueId</v>
-      </c>
-      <c r="O21" s="8">
-        <v>0</v>
-      </c>
-      <c r="P21" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="8" t="str">
+      <c r="M21" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N21" s="7" t="str">
+        <v>FxForward_uniqueId,LUID_XHV68ZZA</v>
+      </c>
+      <c r="O21" s="7" t="str">
         <v>FxForward</v>
+      </c>
+      <c r="P21" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q21" s="1" t="str">
+        <v/>
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -1965,50 +1950,50 @@
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>44512</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <v>44608</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <v>-1000000</v>
       </c>
-      <c r="F22" s="8" t="str">
+      <c r="F22" s="7" t="str">
         <v>EUR</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>1147777</v>
       </c>
-      <c r="H22" s="8" t="str">
+      <c r="H22" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="7">
         <v>1.1448</v>
       </c>
-      <c r="J22" s="8" t="b">
+      <c r="J22" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K22" s="7">
         <v>44607</v>
       </c>
-      <c r="L22" s="8" t="str">
+      <c r="L22" s="7" t="str">
         <v>EUR</v>
       </c>
-      <c r="M22" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N22" s="8" t="str">
-        <v>LUID_T9IFXCOY,InterestRateSwap_uniqueId</v>
-      </c>
-      <c r="O22" s="8">
-        <v>0</v>
-      </c>
-      <c r="P22" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="8" t="str">
+      <c r="M22" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N22" s="7" t="str">
+        <v>InterestRateSwap_uniqueId,LUID_T9IFXCOY</v>
+      </c>
+      <c r="O22" s="7" t="str">
         <v>InterestRateSwap</v>
+      </c>
+      <c r="P22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q22" s="1" t="str">
+        <v/>
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2023,50 +2008,50 @@
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>43868</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>44092</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>-1</v>
       </c>
-      <c r="F23" s="8" t="str">
+      <c r="F23" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>109</v>
       </c>
-      <c r="H23" s="8" t="str">
+      <c r="H23" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="7">
         <v>0</v>
       </c>
-      <c r="J23" s="8" t="b">
+      <c r="J23" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K23" s="7">
         <v>0</v>
       </c>
-      <c r="L23" s="8">
+      <c r="L23" s="7">
         <v>0</v>
       </c>
-      <c r="M23" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N23" s="8" t="str">
-        <v>LUID_PS1AKQYM,id-fxfwd-2</v>
-      </c>
-      <c r="O23" s="8">
-        <v>0</v>
-      </c>
-      <c r="P23" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="8" t="str">
+      <c r="M23" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N23" s="7" t="str">
+        <v>id-fxfwd-2,LUID_PS1AKQYM</v>
+      </c>
+      <c r="O23" s="7" t="str">
         <v>some-name-for-this-fxforward</v>
+      </c>
+      <c r="P23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q23" s="1" t="str">
+        <v/>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -2081,50 +2066,50 @@
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>43868</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="7">
         <v>44092</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>-1</v>
       </c>
-      <c r="F24" s="8" t="str">
+      <c r="F24" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="7">
         <v>109</v>
       </c>
-      <c r="H24" s="8" t="str">
+      <c r="H24" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="7">
         <v>0</v>
       </c>
-      <c r="J24" s="8" t="b">
+      <c r="J24" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24" s="7">
         <v>0</v>
       </c>
-      <c r="L24" s="8">
+      <c r="L24" s="7">
         <v>0</v>
       </c>
-      <c r="M24" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N24" s="8" t="str">
-        <v>LUID_GM2M6MIJ,id-fxfwd-for-pricing</v>
-      </c>
-      <c r="O24" s="8">
-        <v>0</v>
-      </c>
-      <c r="P24" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="8" t="str">
+      <c r="M24" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N24" s="7" t="str">
+        <v>id-fxfwd-for-pricing,LUID_GM2M6MIJ</v>
+      </c>
+      <c r="O24" s="7" t="str">
         <v>some-name-for-this-fxforward</v>
+      </c>
+      <c r="P24" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q24" s="1" t="str">
+        <v/>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2139,50 +2124,50 @@
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>43868</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <v>44092</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <v>-1</v>
       </c>
-      <c r="F25" s="8" t="str">
+      <c r="F25" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="7">
         <v>109</v>
       </c>
-      <c r="H25" s="8" t="str">
+      <c r="H25" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="7">
         <v>0</v>
       </c>
-      <c r="J25" s="8" t="b">
+      <c r="J25" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="7">
         <v>0</v>
       </c>
-      <c r="L25" s="8">
+      <c r="L25" s="7">
         <v>0</v>
       </c>
-      <c r="M25" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N25" s="8" t="str">
-        <v>LUID_38KBBI2D,LUID_00001234</v>
-      </c>
-      <c r="O25" s="8">
-        <v>0</v>
-      </c>
-      <c r="P25" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="8" t="str">
+      <c r="M25" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N25" s="7" t="str">
+        <v>LUID_00001234,LUID_38KBBI2D</v>
+      </c>
+      <c r="O25" s="7" t="str">
         <v>some-name-for-this-fxforward</v>
+      </c>
+      <c r="P25" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q25" s="1" t="str">
+        <v/>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -2197,50 +2182,50 @@
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>44249</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <v>44614</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <v>-1</v>
       </c>
-      <c r="F26" s="8" t="str">
+      <c r="F26" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="7">
         <v>109</v>
       </c>
-      <c r="H26" s="8" t="str">
+      <c r="H26" s="7" t="str">
         <v>JPY</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="7">
         <v>0</v>
       </c>
-      <c r="J26" s="8" t="b">
+      <c r="J26" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="7">
         <v>0</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L26" s="7">
         <v>0</v>
       </c>
-      <c r="M26" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="N26" s="8" t="str">
-        <v>LUID_7KPMGPYY,usd-jpy-fwd</v>
-      </c>
-      <c r="O26" s="8">
-        <v>0</v>
-      </c>
-      <c r="P26" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="8" t="str">
+      <c r="M26" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="N26" s="7" t="str">
+        <v>usd-jpy-fwd,LUID_7KPMGPYY</v>
+      </c>
+      <c r="O26" s="7" t="str">
         <v>some-name-for-this-fxforward</v>
+      </c>
+      <c r="P26" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q26" s="1" t="str">
+        <v/>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -2255,50 +2240,50 @@
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="8" t="str">
+      <c r="C27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="D27" s="8" t="str">
+      <c r="D27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="E27" s="8" t="str">
+      <c r="E27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="F27" s="8" t="str">
+      <c r="F27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="G27" s="8" t="str">
+      <c r="G27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="H27" s="8" t="str">
+      <c r="H27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="I27" s="8" t="str">
+      <c r="I27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="J27" s="8" t="str">
+      <c r="J27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="K27" s="8" t="str">
+      <c r="K27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="L27" s="8" t="str">
+      <c r="L27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="M27" s="8" t="str">
+      <c r="M27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="N27" s="8" t="str">
+      <c r="N27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="O27" s="8" t="str">
+      <c r="O27" s="7" t="str">
         <v>[More...]</v>
       </c>
-      <c r="P27" s="9" t="str">
-        <v>[More...]</v>
-      </c>
-      <c r="Q27" s="8" t="str">
-        <v>[More...]</v>
+      <c r="P27" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Q27" s="1" t="str">
+        <v/>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -2466,12 +2451,8 @@
       <c r="O32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P32" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
@@ -2485,21 +2466,21 @@
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="8"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
@@ -2513,21 +2494,21 @@
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="8"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
@@ -2541,21 +2522,21 @@
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="8"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
@@ -2569,21 +2550,21 @@
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
@@ -2597,21 +2578,21 @@
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
@@ -2625,21 +2606,21 @@
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="8"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
@@ -2653,21 +2634,21 @@
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="8"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
@@ -2681,21 +2662,21 @@
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -2709,21 +2690,21 @@
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
@@ -2795,22 +2776,22 @@
       <c r="Z43" s="1"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="15">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name" sqref="C32" xr:uid="{A1279EB5-614B-4394-8A00-AA32F2E4B821}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Types" sqref="D32" xr:uid="{325D66AF-547B-4A63-BB8B-F160312D5817}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Ids" sqref="E32" xr:uid="{E64BCE8B-D3AC-4268-BB94-ECF82351123D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LookThroughPortfolioId Scope" sqref="F32" xr:uid="{8107FBD1-8557-4D57-BBBB-70A05EDED1AF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LookThroughPortfolioId Code" sqref="G32" xr:uid="{33E90796-7E7D-4A8E-B27C-917BE0E62729}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="StartDate" sqref="H32" xr:uid="{50D2ED42-56E6-409C-9BC4-E44C6CB6AA7F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="MaturityDate" sqref="I32" xr:uid="{791152C1-866D-4FB2-8683-7D0DEECDC9C3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DomAmount" sqref="J32" xr:uid="{88E0C8A9-373B-4E98-98C2-AB6A5B49B7E3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DomCcy" sqref="K32" xr:uid="{64634901-DC08-4F72-B640-CEC1CE520FA5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FgnAmount" sqref="L32" xr:uid="{2348A54C-FE34-49EE-BFE1-029A826E4793}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FgnCcy" sqref="M32" xr:uid="{9213113A-0398-4FC0-A559-8D3F55FD1A74}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="RefSpotRate" sqref="N32" xr:uid="{CC32103D-1FEF-450D-AF76-C58E5441330E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="IsNdf" sqref="O32" xr:uid="{9119B468-A600-4DB3-903F-7E9E878B0981}"/>
+  <dataValidations count="15">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FixingDate" sqref="P32" xr:uid="{2F2105F9-068C-47FC-9681-F303D0090D1B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="SettlementCcy" sqref="Q32" xr:uid="{5F4C1BCF-1DAE-407F-B62A-5CE1C6997A92}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name" sqref="C32" xr:uid="{BD61CCDD-5CE1-491E-8D11-69DB5C10779F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Types" sqref="D32" xr:uid="{DEEAC682-59C8-429D-9278-7A76298A1D8B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Ids" sqref="E32" xr:uid="{A02F9862-D4BE-4BC5-BCD2-DC184AEB5BF3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="StartDate" sqref="F32" xr:uid="{7E337B47-A352-420A-B3BF-3E2195A09566}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="MaturityDate" sqref="G32" xr:uid="{9A946B9C-D7CC-42ED-A3F8-02B651C06B02}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DomAmount" sqref="H32" xr:uid="{52DF61F3-24BB-40C7-997A-B038EBAED45E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="DomCcy" sqref="I32" xr:uid="{4D45BB1D-DF51-405B-9C16-B47D030CCC23}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FgnAmount" sqref="J32" xr:uid="{15480889-C640-4900-B79A-0BCD963F567D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FgnCcy" sqref="K32" xr:uid="{7993F5F2-7963-4DE8-9EA3-0A2941463547}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="RefSpotRate" sqref="L32" xr:uid="{F569D225-F547-446D-8CEF-B734782E6173}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="IsNdf" sqref="M32" xr:uid="{7EF8A577-5C0E-4E71-9193-4B65F9883336}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FixingDate" sqref="N32" xr:uid="{C2B159A6-C107-4770-9AF6-8289B17C4024}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="SettlementCcy" sqref="O32" xr:uid="{31D8D0B2-A37A-43C7-BF00-F6D22D3E9644}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2820,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90759B6D-4CB9-4D5B-BC0B-C7D05AD9C258}">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2920,7 +2901,7 @@
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2953,7 +2934,7 @@
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3048,7 +3029,7 @@
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -3111,7 +3092,7 @@
     </row>
     <row r="9" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5"/>
@@ -3175,7 +3156,7 @@
     </row>
     <row r="11" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="5"/>
@@ -3239,7 +3220,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5"/>
@@ -3403,13 +3384,13 @@
         <v>Instrument Ids</v>
       </c>
       <c r="Y16" s="6" t="str">
-        <v>LookThroughPortfolioId Scope</v>
-      </c>
-      <c r="Z16" s="6" t="str">
-        <v>LookThroughPortfolioId Code</v>
-      </c>
-      <c r="AA16" s="6" t="str">
         <v>Name</v>
+      </c>
+      <c r="Z16" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA16" s="1" t="str">
+        <v/>
       </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
@@ -3417,80 +3398,80 @@
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>43835</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>43866</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>1000000</v>
       </c>
-      <c r="F17" s="8" t="str">
+      <c r="F17" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>-1380000</v>
       </c>
-      <c r="H17" s="8" t="str">
+      <c r="H17" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="7">
         <v>1.38</v>
       </c>
-      <c r="J17" s="8" t="b">
+      <c r="J17" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="7">
         <v>43835</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="7">
         <v>0</v>
       </c>
-      <c r="M17" s="8">
+      <c r="M17" s="7">
         <v>43835</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="7">
         <v>43895</v>
       </c>
-      <c r="O17" s="8">
+      <c r="O17" s="7">
         <v>1000000</v>
       </c>
-      <c r="P17" s="8" t="str">
+      <c r="P17" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="Q17" s="8">
+      <c r="Q17" s="7">
         <v>-1380000</v>
       </c>
-      <c r="R17" s="8" t="str">
+      <c r="R17" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="S17" s="8">
+      <c r="S17" s="7">
         <v>1.38</v>
       </c>
-      <c r="T17" s="8" t="b">
+      <c r="T17" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="U17" s="8">
+      <c r="U17" s="7">
         <v>43835</v>
       </c>
-      <c r="V17" s="8">
+      <c r="V17" s="7">
         <v>0</v>
       </c>
-      <c r="W17" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="X17" s="8" t="str">
-        <v>LUID_00004E5I,id-fx-swap-1</v>
-      </c>
-      <c r="Y17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="8" t="str">
+      <c r="W17" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="X17" s="7" t="str">
+        <v>id-fx-swap-1,LUID_00004E5I</v>
+      </c>
+      <c r="Y17" s="7" t="str">
         <v>ProperlyDefinedFXSwap1</v>
+      </c>
+      <c r="Z17" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA17" s="1" t="str">
+        <v/>
       </c>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
@@ -3498,80 +3479,80 @@
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>43790</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>43970</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>100000000</v>
       </c>
-      <c r="F18" s="8" t="str">
+      <c r="F18" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>-128863000</v>
       </c>
-      <c r="H18" s="8" t="str">
+      <c r="H18" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <v>1.2886299999999999</v>
       </c>
-      <c r="J18" s="8" t="b">
+      <c r="J18" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="7">
         <v>43790</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="7">
         <v>0</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18" s="7">
         <v>43790</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="7">
         <v>43972</v>
       </c>
-      <c r="O18" s="8">
+      <c r="O18" s="7">
         <v>50000000</v>
       </c>
-      <c r="P18" s="8" t="str">
+      <c r="P18" s="7" t="str">
         <v>GBP</v>
       </c>
-      <c r="Q18" s="8">
+      <c r="Q18" s="7">
         <v>-64431500</v>
       </c>
-      <c r="R18" s="8" t="str">
+      <c r="R18" s="7" t="str">
         <v>USD</v>
       </c>
-      <c r="S18" s="8">
+      <c r="S18" s="7">
         <v>1.2886299999999999</v>
       </c>
-      <c r="T18" s="8" t="b">
+      <c r="T18" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="U18" s="8">
+      <c r="U18" s="7">
         <v>43790</v>
       </c>
-      <c r="V18" s="8">
+      <c r="V18" s="7">
         <v>0</v>
       </c>
-      <c r="W18" s="8" t="str">
-        <v>LusidInstrumentId,ClientInternal</v>
-      </c>
-      <c r="X18" s="8" t="str">
-        <v>LUID_00017MQ2,MyExcelSwap</v>
-      </c>
-      <c r="Y18" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="8" t="str">
-        <v>ExcelSwap</v>
+      <c r="W18" s="7" t="str">
+        <v>ClientInternal,LusidInstrumentId</v>
+      </c>
+      <c r="X18" s="7" t="str">
+        <v>MyExcelSwap,LUID_00017MQ2</v>
+      </c>
+      <c r="Y18" s="7" t="str">
+        <v>ExcelSwapUpdate</v>
+      </c>
+      <c r="Z18" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA18" s="1" t="str">
+        <v/>
       </c>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
@@ -3579,79 +3560,79 @@
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z19" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA19" s="8" t="str">
+      <c r="C19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y19" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z19" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA19" s="1" t="str">
         <v/>
       </c>
       <c r="AB19" s="1"/>
@@ -3660,79 +3641,79 @@
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z20" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA20" s="8" t="str">
+      <c r="C20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y20" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z20" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA20" s="1" t="str">
         <v/>
       </c>
       <c r="AB20" s="1"/>
@@ -3741,79 +3722,79 @@
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z21" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA21" s="8" t="str">
+      <c r="C21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y21" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z21" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA21" s="1" t="str">
         <v/>
       </c>
       <c r="AB21" s="1"/>
@@ -3822,79 +3803,79 @@
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z22" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA22" s="8" t="str">
+      <c r="C22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y22" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA22" s="1" t="str">
         <v/>
       </c>
       <c r="AB22" s="1"/>
@@ -3903,79 +3884,79 @@
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z23" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA23" s="8" t="str">
+      <c r="C23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y23" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA23" s="1" t="str">
         <v/>
       </c>
       <c r="AB23" s="1"/>
@@ -3984,79 +3965,79 @@
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z24" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA24" s="8" t="str">
+      <c r="C24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z24" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA24" s="1" t="str">
         <v/>
       </c>
       <c r="AB24" s="1"/>
@@ -4065,79 +4046,79 @@
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z25" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA25" s="8" t="str">
+      <c r="C25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y25" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z25" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA25" s="1" t="str">
         <v/>
       </c>
       <c r="AB25" s="1"/>
@@ -4146,79 +4127,79 @@
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z26" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA26" s="8" t="str">
+      <c r="C26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y26" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z26" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA26" s="1" t="str">
         <v/>
       </c>
       <c r="AB26" s="1"/>
@@ -4227,79 +4208,79 @@
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="D27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="E27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="F27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="G27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="H27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="I27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="J27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="K27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="L27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="M27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="N27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="O27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="P27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Q27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="R27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="S27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="T27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="U27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="V27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="W27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="X27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Y27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="Z27" s="8" t="str">
-        <v/>
-      </c>
-      <c r="AA27" s="8" t="str">
+      <c r="C27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="D27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="E27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="F27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="J27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="M27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="O27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="P27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Q27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="R27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y27" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z27" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA27" s="1" t="str">
         <v/>
       </c>
       <c r="AB27" s="1"/>
@@ -4370,7 +4351,7 @@
     <row r="30" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -4444,10 +4425,10 @@
         <v>9</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>22</v>
@@ -4503,291 +4484,287 @@
       <c r="Y32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Z32" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA32" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="8"/>
-      <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-      <c r="AA34" s="8"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-      <c r="AA37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="8"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="8"/>
-      <c r="AA38" s="8"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-      <c r="AA39" s="8"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-      <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-      <c r="AA40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="8"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-      <c r="AA41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
     </row>
@@ -4859,31 +4836,31 @@
     </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name" sqref="C32" xr:uid="{90964898-6A50-42A4-A407-2C38FCE3163A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Types" sqref="D32" xr:uid="{8AD2BD29-C252-461C-81B8-23C4D02A5783}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Ids" sqref="E32" xr:uid="{74F30A5B-D083-4651-882E-0D8B895BFB72}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LookThroughPortfolioId Scope" sqref="F32" xr:uid="{83AAE353-95AE-4290-B8A6-319A7BC31571}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="LookThroughPortfolioId Code" sqref="G32" xr:uid="{14125927-AE07-4F79-996F-E9F6A78A8C65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearStartDate" sqref="H32" xr:uid="{9853CD87-24C8-4AC9-B27B-381D24CFFBE2}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearMaturityDate" sqref="I32" xr:uid="{35CFF59C-ED80-4384-A2D4-43E09AD39A53}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearDomAmount" sqref="J32" xr:uid="{C1181864-CC7E-4F38-B98E-61F906CC2D87}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearDomCcy" sqref="K32" xr:uid="{150AD7C1-F6AA-4784-83E1-8D7F6253EFFF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFgnAmount" sqref="L32" xr:uid="{1C702FD4-DB49-4B51-8F04-F5C31A66EF65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFgnCcy" sqref="M32" xr:uid="{728AC5BF-C083-45B1-8ABC-DF3FB67C1D65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearRefSpotRate" sqref="N32" xr:uid="{41D0F7CA-CB1A-452C-8CAC-58DB797F2B79}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearIsNdf" sqref="O32" xr:uid="{52F9125E-7702-434A-AC65-9E60FACE62DA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFixingDate" sqref="P32" xr:uid="{19CF1615-0B9F-4FA3-BB5C-49F569ABF2AB}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearSettlementCcy" sqref="Q32" xr:uid="{725661D4-958D-49D6-902A-C4DDBA6A3163}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarStartDate" sqref="R32" xr:uid="{CEE78929-9A41-44EB-9F43-5AD06462B324}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarMaturityDate" sqref="S32" xr:uid="{F42348B6-3041-4AE2-9E68-07F0237A083E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarDomAmount" sqref="T32" xr:uid="{8883C7AF-3463-4C9B-9330-9AE7EDCBBD56}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarDomCcy" sqref="U32" xr:uid="{2DC41E1E-4302-4BE1-9CDA-4BFFD4785D56}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFgnAmount" sqref="V32" xr:uid="{E4D796FC-0F15-49D8-B27A-0D2E81D45132}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFgnCcy" sqref="W32" xr:uid="{E9BD797A-7F53-4C61-9828-766BEDFAD568}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarRefSpotRate" sqref="X32" xr:uid="{CF405A83-357D-4F4F-92B5-334D82BC67B4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarIsNdf" sqref="Y32" xr:uid="{039641DE-88AB-4A09-A04E-26869758AE4F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFixingDate" sqref="Z32" xr:uid="{51D3CF76-0FF8-415C-AA02-08414034D391}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarSettlementCcy" sqref="AA32" xr:uid="{BC24EC2D-82E8-49E3-B152-56AC8D6353AF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name" sqref="C32" xr:uid="{C0606741-901B-4788-A8C4-DF4BA9A21AD5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Id Types" sqref="D32" xr:uid="{8E69A5A4-CC06-4CAC-9639-B3E2E010134F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Instrument Ids" sqref="E32" xr:uid="{E3AF64E3-8B39-4BCC-A8E7-E49F5E092CB6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearStartDate" sqref="F32" xr:uid="{DAC9DFEB-7577-48B9-8EFF-E21B89A2AF6C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearMaturityDate" sqref="G32" xr:uid="{9919D987-07C2-4504-B1D2-BED99EA34AEE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearDomAmount" sqref="H32" xr:uid="{C0FDD185-D37C-49E0-9A64-EA6C3468D97B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearDomCcy" sqref="I32" xr:uid="{411BD543-E23F-41B4-96EE-342DE512C11E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFgnAmount" sqref="J32" xr:uid="{A926503F-88F1-43B7-82E9-E8D1D8E5A73D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFgnCcy" sqref="K32" xr:uid="{3FDDB716-6D74-4721-9F43-11717312EA25}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearRefSpotRate" sqref="L32" xr:uid="{AF749B97-71F8-43E8-A544-4F82DE8BC690}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearIsNdf" sqref="M32" xr:uid="{6669FAD6-D630-45AB-8DEF-6D06173B361E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearFixingDate" sqref="N32" xr:uid="{FD81C621-CDFF-4A76-B24B-1FBD986FE6BA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="NearSettlementCcy" sqref="O32" xr:uid="{DDF52DC9-0DF6-46EC-9DD4-728BCA7031DD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarStartDate" sqref="P32" xr:uid="{94E081C3-A528-470F-9A3B-A2450C5EC3E2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarMaturityDate" sqref="Q32" xr:uid="{EA7F0344-4D49-43BA-A278-A14F79732AD5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarDomAmount" sqref="R32" xr:uid="{AE0FC776-F139-4CB3-8F0F-EA34876D53C3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarDomCcy" sqref="S32" xr:uid="{9022B845-CFC4-4D5B-89B4-D0FFECDA5B54}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFgnAmount" sqref="T32" xr:uid="{951D9CEF-8D51-45F1-B118-96404C02E269}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFgnCcy" sqref="U32" xr:uid="{6764D403-3C60-4F6E-BC5E-40BF55CF530D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarRefSpotRate" sqref="V32" xr:uid="{8CE66E50-5FAF-4DF9-B1BA-FED7D6FF4BFC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarIsNdf" sqref="W32" xr:uid="{0E36B9A2-C13F-4BA9-9F8B-8A356CAC9C49}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarFixingDate" sqref="X32" xr:uid="{43395E3B-F6E9-446A-845A-E9F506070B52}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="FarSettlementCcy" sqref="Y32" xr:uid="{06A92193-7ED0-425E-A154-3AB964954CEA}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>